<commit_message>
Second half of ordered brackets chapter
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\Thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECBF144-1B01-4D0C-A456-53F8D053F4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE65FBBB-8E2F-4060-A43B-16FA37A1A4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="9" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="14" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Sheet11" sheetId="12" r:id="rId12"/>
     <sheet name="Sheet12" sheetId="13" r:id="rId13"/>
     <sheet name="Sheet13" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Georgia</t>
   </si>
@@ -236,12 +237,30 @@
   <si>
     <t>C</t>
   </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>m+1</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +282,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Rage Italic"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="7">
@@ -303,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -585,11 +610,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -676,8 +710,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -686,25 +735,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1194,7 +1229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075732FB-7749-402F-AAF5-F378F2F73D43}">
   <dimension ref="B3:AE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -2349,7 +2384,7 @@
   <dimension ref="C7:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:J15"/>
+      <selection activeCell="C10" sqref="C10:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2368,13 +2403,13 @@
     <row r="8" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="62" t="s">
         <v>59</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="70" t="s">
+      <c r="I8" s="62" t="s">
         <v>60</v>
       </c>
       <c r="J8" s="1"/>
@@ -2402,7 +2437,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="69"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="1"/>
@@ -2417,10 +2452,10 @@
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="69"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="69"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="6">
         <v>2</v>
       </c>
@@ -2430,7 +2465,7 @@
       <c r="H12" s="11"/>
       <c r="I12" s="6"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="69"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="1"/>
@@ -2443,7 +2478,7 @@
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="20"/>
-      <c r="K13" s="69"/>
+      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
@@ -2456,25 +2491,25 @@
       <c r="H14" s="7"/>
       <c r="I14" s="6"/>
       <c r="J14" s="21"/>
-      <c r="K14" s="69"/>
+      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6">
         <v>3</v>
       </c>
       <c r="I15" s="20"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="69"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="3:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="11"/>
@@ -2487,10 +2522,10 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="72" t="s">
+      <c r="G17" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="71"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="1"/>
@@ -2501,7 +2536,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="71"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="1"/>
@@ -2600,7 +2635,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="71"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
@@ -2702,7 +2737,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="20"/>
-      <c r="I12" s="71"/>
+      <c r="I12" s="6"/>
       <c r="J12" s="11"/>
       <c r="K12" s="6"/>
     </row>
@@ -2758,6 +2793,143 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E2B15B-BC8E-45EF-98BA-5812B803929B}">
+  <dimension ref="C7:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="72"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="71"/>
+    </row>
+    <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="71"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="72"/>
+    </row>
+    <row r="12" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="71"/>
+      <c r="D13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="72"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="71"/>
+    </row>
+    <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="71"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="72"/>
+    </row>
+    <row r="19" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="3:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C20" s="71"/>
+      <c r="D20" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D17:D18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6541,7 +6713,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="62"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -6549,7 +6721,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="62"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="8" t="s">
         <v>27</v>
       </c>
@@ -6583,7 +6755,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="62"/>
+      <c r="D12" s="64"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -6591,7 +6763,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="62"/>
+      <c r="D13" s="64"/>
       <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
@@ -6625,7 +6797,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="62"/>
+      <c r="D16" s="64"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -6633,7 +6805,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="62"/>
+      <c r="D17" s="64"/>
       <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
@@ -6729,7 +6901,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="62"/>
+      <c r="D8" s="64"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -6739,7 +6911,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="62"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -6749,32 +6921,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="66" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="65"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="65"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="68"/>
+      <c r="E12" s="65"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -6782,37 +6954,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="66" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="68"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="63" t="s">
+      <c r="I13" s="68" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="67"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="70"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="63"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="67"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="70"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="64"/>
+      <c r="I15" s="69"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -6821,7 +6993,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="62"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -6831,7 +7003,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="62"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="1" t="s">
         <v>41</v>
       </c>
@@ -6869,9 +7041,9 @@
         <v>38</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -6879,9 +7051,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
       <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
@@ -6900,17 +7072,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Closes #1 and #2
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F7897-29F0-4D84-B14E-CA7CBEC9A1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BA62B1-5946-4474-AFE8-2ABE20DE835F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="7" activeTab="15" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="7" activeTab="16" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -770,7 +770,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -779,21 +782,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2431,7 +2427,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="70" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="1"/>
@@ -2440,7 +2436,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -2486,7 +2482,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="70" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="1"/>
@@ -2495,7 +2491,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -3102,36 +3098,48 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC68B215-176C-47A9-BC65-E5FAC0AEE706}">
-  <dimension ref="B2:N19"/>
+  <dimension ref="B2:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-    </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+    </row>
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="58"/>
-      <c r="N3" s="74"/>
-    </row>
-    <row r="4" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="6">
         <v>1</v>
@@ -3139,27 +3147,43 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="74"/>
-    </row>
-    <row r="5" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74">
+        <v>1</v>
+      </c>
+      <c r="T4" s="74"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="66"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="58"/>
-      <c r="N5" s="74"/>
-    </row>
-    <row r="6" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <v>6</v>
+      </c>
+      <c r="S5" s="11"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="8">
         <v>8</v>
@@ -3167,139 +3191,213 @@
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
-      <c r="I6" s="74"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="74"/>
-    </row>
-    <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="6"/>
       <c r="D7" s="59"/>
       <c r="E7" s="5"/>
       <c r="F7" s="1"/>
-      <c r="I7" s="74"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="58"/>
-      <c r="N7" s="74"/>
-    </row>
-    <row r="8" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="12">
+        <v>7</v>
+      </c>
+      <c r="S7" s="20"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="6">
         <v>4</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="74"/>
-      <c r="I8" s="74"/>
+      <c r="F8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="74"/>
-    </row>
-    <row r="9" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="74">
+        <v>2</v>
+      </c>
+      <c r="T8" s="74"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="66"/>
       <c r="D9" s="1"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="74"/>
-      <c r="I9" s="74"/>
+      <c r="F9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="74"/>
-    </row>
-    <row r="10" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6">
+        <v>5</v>
+      </c>
+      <c r="S9" s="11"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="8">
         <v>5</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="74"/>
-      <c r="I10" s="74"/>
+      <c r="F10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="74"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="6"/>
       <c r="D11" s="1"/>
       <c r="E11" s="59"/>
-      <c r="F11" s="74"/>
-      <c r="I11" s="74"/>
+      <c r="F11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="3"/>
       <c r="K11" s="4"/>
       <c r="L11" s="1"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="74"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="12">
+        <v>8</v>
+      </c>
+      <c r="S11" s="20"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="6">
         <v>3</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="74"/>
-      <c r="I12" s="74"/>
+      <c r="F12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="74"/>
-    </row>
-    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="74">
+        <v>3</v>
+      </c>
+      <c r="T12" s="74"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="66"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="74"/>
-      <c r="I13" s="74"/>
+      <c r="F13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="2"/>
       <c r="L13" s="1"/>
       <c r="M13" s="5"/>
-      <c r="N13" s="74"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="74">
+        <v>4</v>
+      </c>
+      <c r="S13" s="11"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="8">
         <v>6</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="74"/>
-      <c r="I14" s="74"/>
+      <c r="F14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="L14" s="4"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="74"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="6">
+        <v>9</v>
+      </c>
+      <c r="R14" s="7"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="6"/>
       <c r="D15" s="59"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="74"/>
-      <c r="I15" s="74"/>
+      <c r="F15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="3"/>
       <c r="K15" s="4"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="74"/>
-    </row>
-    <row r="16" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="6">
         <v>2</v>
@@ -3307,27 +3405,41 @@
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
       <c r="F16" s="1"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="74"/>
-    </row>
-    <row r="17" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="12">
+        <v>10</v>
+      </c>
+      <c r="R16" s="20"/>
+      <c r="S16" s="74"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="66"/>
       <c r="D17" s="1"/>
       <c r="E17" s="5"/>
       <c r="F17" s="1"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="74"/>
-    </row>
-    <row r="18" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="8">
         <v>7</v>
@@ -3335,25 +3447,37 @@
       <c r="D18" s="4"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="74"/>
-    </row>
-    <row r="19" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="74"/>
+      <c r="N19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3362,12 +3486,96 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C06664-9D9D-4861-B1E9-94FF6B95C706}">
-  <dimension ref="A1"/>
+  <dimension ref="C4:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="10" width="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7360,32 +7568,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="69"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="68"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="70"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="68"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -7393,37 +7601,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="70" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="68"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="71" t="s">
+      <c r="I13" s="68" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="73"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="71"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="73"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="72"/>
+      <c r="I15" s="69"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -7511,17 +7719,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed refactoring on brackets/shapes/signatures!
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D9037B-E8AD-41C5-9DC8-D76E8A653790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D855EFB-7B45-4850-A8F3-F62BA2CBE58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet5 (2)" sheetId="11" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet11" sheetId="12" r:id="rId11"/>
-    <sheet name="Sheet12" sheetId="13" r:id="rId12"/>
-    <sheet name="Sheet13" sheetId="14" r:id="rId13"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId14"/>
-    <sheet name="Sheet15" sheetId="16" r:id="rId15"/>
-    <sheet name="Sheet8" sheetId="17" r:id="rId16"/>
-    <sheet name="Sheet16" sheetId="18" r:id="rId17"/>
+    <sheet name="Sheet17" sheetId="19" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet5 (2)" sheetId="11" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId11"/>
+    <sheet name="Sheet11" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet12" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet13" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet15" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet8" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet16" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -676,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -779,7 +780,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -788,15 +792,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1119,7 +1121,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="A19" sqref="A19:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1345,6 +1347,459 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075732FB-7749-402F-AAF5-F378F2F73D43}">
+  <dimension ref="B3:AE20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7:M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6">
+        <v>1</v>
+      </c>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
+        <v>5</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="19"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6">
+        <v>8</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="19"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6">
+        <v>4</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="19"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="12">
+        <v>11</v>
+      </c>
+      <c r="T8" s="20"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="19"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6">
+        <v>4</v>
+      </c>
+      <c r="U9" s="6"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="6"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="8">
+        <v>5</v>
+      </c>
+      <c r="L10" s="20"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="19"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6">
+        <v>9</v>
+      </c>
+      <c r="T10" s="7"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="6"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="7"/>
+    </row>
+    <row r="11" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6">
+        <v>2</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="19"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="6"/>
+      <c r="AC11" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="58"/>
+    </row>
+    <row r="12" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6">
+        <v>3</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="19"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="12">
+        <v>10</v>
+      </c>
+      <c r="T12" s="20"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="6"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="20"/>
+    </row>
+    <row r="13" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="6">
+        <v>6</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="19"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6">
+        <v>2</v>
+      </c>
+      <c r="W13" s="6"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="6"/>
+      <c r="AC13" s="58">
+        <v>7</v>
+      </c>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="1"/>
+    </row>
+    <row r="14" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="19"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6">
+        <v>3</v>
+      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8">
+        <v>7</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="19"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6">
+        <v>6</v>
+      </c>
+      <c r="U15" s="7"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="19"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="2:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="19"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="12">
+        <v>7</v>
+      </c>
+      <c r="U17" s="20"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C071CB8-4A62-48A5-9C91-383608FE5F7C}">
   <dimension ref="A5:R18"/>
   <sheetViews>
@@ -1575,7 +2030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D228CAD8-B85C-426E-AD63-CE67C9560447}">
   <dimension ref="B5:Q29"/>
   <sheetViews>
@@ -2045,7 +2500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713F1397-54B0-4865-93E4-0B940AD31719}">
   <dimension ref="C7:K26"/>
   <sheetViews>
@@ -2313,7 +2768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AADE0C-132A-4EF3-A172-B6CF6F69AB44}">
   <dimension ref="B7:K16"/>
   <sheetViews>
@@ -2462,7 +2917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E2B15B-BC8E-45EF-98BA-5812B803929B}">
   <dimension ref="C7:G21"/>
   <sheetViews>
@@ -2497,7 +2952,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="70" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -2506,7 +2961,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -2552,7 +3007,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="70" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -2561,7 +3016,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -2599,7 +3054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
   <dimension ref="B4:R28"/>
   <sheetViews>
@@ -3166,7 +3621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC68B215-176C-47A9-BC65-E5FAC0AEE706}">
   <dimension ref="B2:U19"/>
   <sheetViews>
@@ -3554,7 +4009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C06664-9D9D-4861-B1E9-94FF6B95C706}">
   <dimension ref="C4:J6"/>
   <sheetViews>
@@ -3654,7 +4109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D179F0-AC46-41D9-873C-B2A647CFC02F}">
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3842,6 +4297,171 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94C50A0-9EC1-4FB8-9BAB-7873F6DA654A}">
+  <dimension ref="B5:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="6">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="6">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="8">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="8">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="6">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="8">
+        <v>4</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1876FCB-6DB9-423A-8CE5-BFA1290FCF13}">
   <dimension ref="A2:P18"/>
   <sheetViews>
@@ -4218,7 +4838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492D4744-2D7C-45B9-9C52-AF2B5242534C}">
   <dimension ref="A5:K16"/>
   <sheetViews>
@@ -4389,7 +5009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C59F7E8-88AA-4FE9-B6FA-71F38FE540A6}">
   <dimension ref="A4:AA38"/>
   <sheetViews>
@@ -5963,7 +6583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89773F7F-4D17-4965-AFCD-3A60B3CB582B}">
   <dimension ref="A4:Y38"/>
   <sheetViews>
@@ -7368,7 +7988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4FDA5A-1FA6-4FB5-874D-8ADC03C2B365}">
   <dimension ref="B4:G18"/>
   <sheetViews>
@@ -7547,7 +8167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426E89DE-FB26-4184-BD37-CBFF7802F4CC}">
   <dimension ref="B4:I22"/>
   <sheetViews>
@@ -7638,32 +8258,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="70" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="69"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="68"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="70"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="68"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -7671,37 +8291,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="70" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="68"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="71" t="s">
+      <c r="I13" s="68" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="73"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="71"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="73"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="72"/>
+      <c r="I15" s="69"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -7789,471 +8409,18 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075732FB-7749-402F-AAF5-F378F2F73D43}">
-  <dimension ref="B3:AE20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:M11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6">
-        <v>1</v>
-      </c>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6">
-        <v>5</v>
-      </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="19"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6">
-        <v>8</v>
-      </c>
-      <c r="T6" s="7"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6">
-        <v>1</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="19"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6">
-        <v>4</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="19"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="12">
-        <v>11</v>
-      </c>
-      <c r="T8" s="20"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="21"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="6"/>
-    </row>
-    <row r="9" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="19"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6">
-        <v>4</v>
-      </c>
-      <c r="U9" s="6"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="6"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="8">
-        <v>5</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="19"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6">
-        <v>9</v>
-      </c>
-      <c r="T10" s="7"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="6"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1">
-        <v>3</v>
-      </c>
-      <c r="AE10" s="7"/>
-    </row>
-    <row r="11" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
-        <v>2</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6">
-        <v>2</v>
-      </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="19"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="6"/>
-      <c r="AC11" s="1">
-        <v>6</v>
-      </c>
-      <c r="AD11" s="7"/>
-      <c r="AE11" s="58"/>
-    </row>
-    <row r="12" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
-        <v>3</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6">
-        <v>3</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="19"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="12">
-        <v>10</v>
-      </c>
-      <c r="T12" s="20"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="6"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="58"/>
-      <c r="AE12" s="20"/>
-    </row>
-    <row r="13" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="6">
-        <v>6</v>
-      </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="19"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6">
-        <v>2</v>
-      </c>
-      <c r="W13" s="6"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="6"/>
-      <c r="AC13" s="58">
-        <v>7</v>
-      </c>
-      <c r="AD13" s="20"/>
-      <c r="AE13" s="1"/>
-    </row>
-    <row r="14" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="19"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6">
-        <v>3</v>
-      </c>
-      <c r="V14" s="7"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="6"/>
-    </row>
-    <row r="15" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3">
-        <v>11</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="8">
-        <v>7</v>
-      </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="19"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6">
-        <v>6</v>
-      </c>
-      <c r="U15" s="7"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-    </row>
-    <row r="16" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="19"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-    </row>
-    <row r="17" spans="2:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="19"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="12">
-        <v>7</v>
-      </c>
-      <c r="U17" s="20"/>
-      <c r="V17" s="6"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-    </row>
-    <row r="18" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-    </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-    </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to ordered brackets in new style
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D855EFB-7B45-4850-A8F3-F62BA2CBE58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCDF595-69F4-41A8-8F45-DCDAA84A84C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -280,34 +280,34 @@
     <t>3 TCU</t>
   </si>
   <si>
-    <t>1 Gonzaga</t>
+    <t>1 Saint Mary's</t>
   </si>
   <si>
-    <t>4 Santa Clara</t>
+    <t>2 Gonzaga</t>
   </si>
   <si>
-    <t>3 Loyola Marymount</t>
+    <t>3 Santa Clara</t>
   </si>
   <si>
-    <t>2 Saint Mary's</t>
+    <t>4 Loyola Marymount</t>
   </si>
   <si>
-    <t>5 San Francisco</t>
+    <t>5 BYU</t>
   </si>
   <si>
-    <t>6 BYU</t>
+    <t>6 San Francisco</t>
   </si>
   <si>
-    <t>7 Portland</t>
+    <t>7 Pacific</t>
   </si>
   <si>
-    <t>10 San Diego</t>
+    <t>10 Pepperdine</t>
   </si>
   <si>
-    <t>8 Pacific</t>
+    <t>8 Portland</t>
   </si>
   <si>
-    <t>9 Pepperdine</t>
+    <t>9 San Diego</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -780,10 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -792,13 +789,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2952,7 +2951,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="69" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -2961,7 +2960,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="71"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3007,7 +3006,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="69" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3016,7 +3015,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="71"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -4109,13 +4108,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D179F0-AC46-41D9-873C-B2A647CFC02F}">
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -4134,7 +4133,7 @@
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4156,7 +4155,7 @@
     <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
@@ -4169,7 +4168,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
@@ -4182,7 +4181,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1"/>
@@ -4195,7 +4194,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -4217,7 +4216,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="4"/>
@@ -4228,7 +4227,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1"/>
@@ -4239,7 +4238,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
@@ -4250,7 +4249,7 @@
     <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
@@ -4272,7 +4271,7 @@
     <row r="15" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -4300,7 +4299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94C50A0-9EC1-4FB8-9BAB-7873F6DA654A}">
   <dimension ref="B5:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
@@ -4432,12 +4431,12 @@
     </row>
     <row r="13" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="74"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="9"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="74"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="9"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -8258,32 +8257,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="69" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="70"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="68"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="71"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="73"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -8291,37 +8290,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="69" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="73"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="71" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="72"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="68"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="72"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="69"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -8409,17 +8408,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor to three-pronged definition of bracket.
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCDF595-69F4-41A8-8F45-DCDAA84A84C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663FC631-C17C-41B7-9304-E59E2DFE391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -789,13 +792,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1117,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A66EB4-ADAC-4EF1-9D1A-8697917A8679}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1260,7 +1260,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>74</v>
@@ -1269,14 +1269,19 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="6">
         <v>1</v>
@@ -1284,15 +1289,27 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F19" s="1"/>
+      <c r="G19" s="6">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="7"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F20" s="1"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="8">
         <v>4</v>
@@ -1300,15 +1317,27 @@
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F21" s="1"/>
+      <c r="G21" s="8">
+        <v>2</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="6"/>
       <c r="C22" s="1"/>
       <c r="D22" s="5"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="1"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="6">
         <v>2</v>
@@ -1316,15 +1345,27 @@
       <c r="C23" s="1"/>
       <c r="D23" s="4"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F23" s="1"/>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="7"/>
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="1"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="8">
         <v>3</v>
@@ -1332,13 +1373,25 @@
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="1"/>
+      <c r="G25" s="8">
+        <v>4</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2951,7 +3004,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="70" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -2960,7 +3013,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="70"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3006,7 +3059,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="70" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3015,7 +3068,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -4108,7 +4161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D179F0-AC46-41D9-873C-B2A647CFC02F}">
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -8257,32 +8310,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="70" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="69"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="68"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="70"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="68"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -8290,37 +8343,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="70" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="68"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="71" t="s">
+      <c r="I13" s="68" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="73"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="72"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="71"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="73"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="72"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="72"/>
+      <c r="I15" s="69"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -8408,17 +8461,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First attempt at multiple elimination chapter
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663FC631-C17C-41B7-9304-E59E2DFE391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FA14FF-9366-4CA6-8C3F-91E92F221386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="8" activeTab="15" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
   <si>
     <t>Georgia</t>
   </si>
@@ -223,24 +223,12 @@
     <t>South Korea</t>
   </si>
   <si>
-    <t>Uzbekistan</t>
-  </si>
-  <si>
-    <t>Iran</t>
-  </si>
-  <si>
     <t>Iraq</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>Japan</t>
-  </si>
-  <si>
     <t>UAE</t>
   </si>
   <si>
@@ -308,6 +296,42 @@
   </si>
   <si>
     <t>9 San Diego</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>1 South Korea</t>
+  </si>
+  <si>
+    <t>8 Uzbekistan</t>
+  </si>
+  <si>
+    <t>4 Iran</t>
+  </si>
+  <si>
+    <t>5 Iraq</t>
+  </si>
+  <si>
+    <t>3 China</t>
+  </si>
+  <si>
+    <t>6 Australia</t>
+  </si>
+  <si>
+    <t>2 Japan</t>
+  </si>
+  <si>
+    <t>7 UAE</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -780,10 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -792,10 +813,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1119,7 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A66EB4-ADAC-4EF1-9D1A-8697917A8679}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -1138,7 +1162,7 @@
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1156,7 +1180,7 @@
     <row r="4" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
@@ -1174,7 +1198,7 @@
     <row r="6" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="4"/>
@@ -1192,7 +1216,7 @@
     <row r="8" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1"/>
@@ -1215,7 +1239,7 @@
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1231,7 +1255,7 @@
     <row r="13" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
@@ -1247,7 +1271,7 @@
     <row r="15" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="4"/>
@@ -1263,7 +1287,7 @@
     <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1"/>
@@ -1402,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075732FB-7749-402F-AAF5-F378F2F73D43}">
   <dimension ref="B3:AE20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="K7" sqref="K7:M11"/>
     </sheetView>
   </sheetViews>
@@ -2086,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D228CAD8-B85C-426E-AD63-CE67C9560447}">
   <dimension ref="B5:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
@@ -3004,7 +3028,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="69" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3013,7 +3037,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="71"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3059,7 +3083,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="69" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3068,7 +3092,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="71"/>
+      <c r="D18" s="70"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -3108,20 +3132,21 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
-  <dimension ref="B4:R28"/>
+  <dimension ref="B4:AD28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="C6:F19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3139,32 +3164,64 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="6" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="6"/>
+      <c r="N5" s="6">
+        <v>1</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S5" s="6">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="66" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3179,39 +3236,75 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="66" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S6" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+    </row>
+    <row r="7" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8">
+        <v>8</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="8" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="8">
+        <v>8</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S7" s="8">
+        <v>8</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="8">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+    </row>
+    <row r="8" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
       <c r="D8" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1"/>
@@ -3226,37 +3319,73 @@
       <c r="M8" s="1"/>
       <c r="N8" s="6"/>
       <c r="O8" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S8" s="6"/>
+      <c r="T8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+    </row>
+    <row r="9" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>4</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="1"/>
       <c r="H9" s="6" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="6"/>
+      <c r="N9" s="6">
+        <v>4</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S9" s="6">
+        <v>4</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="6">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+    </row>
+    <row r="10" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="66" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="5"/>
@@ -3264,47 +3393,83 @@
       <c r="G10" s="1"/>
       <c r="H10" s="7"/>
       <c r="I10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="66" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+    </row>
+    <row r="11" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="1"/>
       <c r="F11" s="5"/>
       <c r="G11" s="1"/>
       <c r="H11" s="8" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="1"/>
       <c r="K11" s="5"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="8"/>
+      <c r="N11" s="8">
+        <v>5</v>
+      </c>
       <c r="O11" s="4"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S11" s="8">
+        <v>5</v>
+      </c>
+      <c r="T11" s="4"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="8">
+        <v>5</v>
+      </c>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+    </row>
+    <row r="12" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
       <c r="E12" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="1"/>
@@ -3312,43 +3477,79 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="6"/>
       <c r="O12" s="1"/>
       <c r="P12" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S12" s="6"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="V12" s="5"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+    </row>
+    <row r="13" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6">
+        <v>3</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="6" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="4"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="6"/>
+      <c r="N13" s="6">
+        <v>3</v>
+      </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S13" s="6">
+        <v>3</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="6">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+    </row>
+    <row r="14" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="66" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -3356,46 +3557,82 @@
       <c r="G14" s="1"/>
       <c r="H14" s="7"/>
       <c r="I14" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="5"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="66" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S14" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+    </row>
+    <row r="15" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="8"/>
+      <c r="C15" s="8">
+        <v>6</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="1"/>
       <c r="H15" s="8" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="8"/>
+      <c r="N15" s="8">
+        <v>6</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="1"/>
-    </row>
-    <row r="16" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S15" s="8">
+        <v>6</v>
+      </c>
+      <c r="T15" s="4"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="8">
+        <v>6</v>
+      </c>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+    </row>
+    <row r="16" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="6"/>
       <c r="D16" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -3403,44 +3640,80 @@
       <c r="H16" s="6"/>
       <c r="I16" s="1"/>
       <c r="J16" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="6"/>
       <c r="O16" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S16" s="6"/>
+      <c r="T16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+    </row>
+    <row r="17" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="4"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="6" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="4"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="6"/>
+      <c r="N17" s="6">
+        <v>2</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S17" s="6">
+        <v>2</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="6">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+    </row>
+    <row r="18" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="66" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="5"/>
@@ -3450,54 +3723,92 @@
         <v>9</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="66" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+    </row>
+    <row r="19" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8">
+        <v>7</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="8" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="8"/>
+      <c r="N19" s="8">
+        <v>7</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S19" s="8">
+        <v>7</v>
+      </c>
+      <c r="T19" s="4"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="8">
+        <v>7</v>
+      </c>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+    </row>
+    <row r="20" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -3505,17 +3816,35 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="V20" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+    </row>
+    <row r="21" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="66" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3523,31 +3852,49 @@
       <c r="I21" s="1"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="66" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="V21" s="8"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA21" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+    </row>
+    <row r="22" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="1"/>
@@ -3555,12 +3902,28 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q22" s="4"/>
       <c r="R22" s="1"/>
-    </row>
-    <row r="23" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V22" s="4"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="1"/>
+    </row>
+    <row r="23" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -3578,8 +3941,24 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="1"/>
+    </row>
+    <row r="24" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -3597,8 +3976,22 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="1"/>
+    </row>
+    <row r="25" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -3616,8 +4009,24 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="1"/>
+    </row>
+    <row r="26" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -3635,8 +4044,22 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+    </row>
+    <row r="27" spans="2:30" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -3654,8 +4077,22 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+    </row>
+    <row r="28" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -3667,6 +4104,24 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4186,7 +4641,7 @@
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4208,7 +4663,7 @@
     <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
@@ -4221,7 +4676,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
@@ -4234,7 +4689,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1"/>
@@ -4247,7 +4702,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -4269,7 +4724,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="4"/>
@@ -4280,7 +4735,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1"/>
@@ -4291,7 +4746,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
@@ -4302,7 +4757,7 @@
     <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
@@ -4324,7 +4779,7 @@
     <row r="15" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -8310,32 +8765,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="69" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="70"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="68"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="71"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="73"/>
+      <c r="E12" s="68"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -8343,37 +8798,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="69" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="73"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="71" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="72"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="68"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="72"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="69"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -8461,17 +8916,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First draft of swiss complete (needs lots of work obv)
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\Brackets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5736D71-255E-4DA0-A067-5C94B8B9C9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6971372-E574-421E-8517-20E75F8344E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="11" activeTab="20" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="21" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="Sheet18" sheetId="20" r:id="rId19"/>
     <sheet name="Sheet19" sheetId="21" r:id="rId20"/>
     <sheet name="Sheet20" sheetId="22" r:id="rId21"/>
+    <sheet name="Sheet21" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -909,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1024,6 +1025,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1050,10 +1062,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3261,7 +3269,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="84" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3270,7 +3278,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="78"/>
+      <c r="D11" s="85"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3316,7 +3324,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="77" t="s">
+      <c r="D17" s="84" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3325,7 +3333,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="78"/>
+      <c r="D18" s="85"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -6851,7 +6859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D84D55B-86DB-41A7-86B6-8D3E6C4FEE99}">
   <dimension ref="C4:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E14" sqref="E14:H28"/>
     </sheetView>
   </sheetViews>
@@ -6872,16 +6880,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="88" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="82"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="67"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="81" t="s">
+      <c r="H5" s="88" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="82"/>
+      <c r="I5" s="89"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -7415,7 +7423,7 @@
   <dimension ref="A4:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C14"/>
+      <selection activeCell="E6" sqref="C6:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7991,7 +7999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DAA05C-8B34-498C-B0AB-56B73244FFB8}">
   <dimension ref="A4:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
@@ -8019,434 +8027,434 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="83"/>
-      <c r="B10" s="83"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="83"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="83"/>
-      <c r="B12" s="83"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="83"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="83"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
-      <c r="L14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="83"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="83"/>
-      <c r="N15" s="83"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="83"/>
-      <c r="B16" s="83"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="83"/>
-      <c r="M16" s="83"/>
-      <c r="N16" s="83"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="83"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
-      <c r="N17" s="83"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
-      <c r="B18" s="83"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="83"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="83"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="83"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="83"/>
-      <c r="B22" s="83"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="66" t="s">
         <v>59</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
       <c r="H22" s="66" t="s">
         <v>59</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="J22" s="83"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="8" t="s">
         <v>123</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
       <c r="H23" s="8" t="s">
         <v>123</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="83"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="83"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="83"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="83"/>
-      <c r="B26" s="83"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84" t="s">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="J26" s="83"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="83"/>
-      <c r="N26" s="83"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="83"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="84" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D27" s="66" t="s">
         <v>65</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="84" t="s">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="6" t="s">
         <v>124</v>
       </c>
       <c r="I27" s="66" t="s">
@@ -8455,22 +8463,22 @@
       <c r="J27" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K27" s="83"/>
-      <c r="L27" s="83"/>
-      <c r="M27" s="83"/>
-      <c r="N27" s="83"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="83"/>
-      <c r="B28" s="83"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="66" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="66" t="s">
         <v>63</v>
       </c>
@@ -8478,99 +8486,1222 @@
         <v>128</v>
       </c>
       <c r="J28" s="4"/>
-      <c r="K28" s="83"/>
-      <c r="L28" s="83"/>
-      <c r="M28" s="83"/>
-      <c r="N28" s="83"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="83"/>
-      <c r="B29" s="83"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="8" t="s">
         <v>125</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="8" t="s">
         <v>125</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="J29" s="83"/>
-      <c r="K29" s="83"/>
-      <c r="L29" s="83"/>
-      <c r="M29" s="83"/>
-      <c r="N29" s="83"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="83"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="83"/>
-      <c r="N30" s="83"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="83"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="83"/>
-      <c r="N31" s="83"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="83"/>
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="83"/>
-      <c r="N32" s="83"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83"/>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="83"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FC37AD-F8C8-422A-907B-37F83257262D}">
+  <dimension ref="A3:AB94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC71" sqref="Z71:AC83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>SUM(C3:ZZ3)</f>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A18" si="0">SUM(C4:ZZ4)</f>
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B18" si="1">B4+1</f>
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="Q21" s="74"/>
+      <c r="X21" s="74"/>
+    </row>
+    <row r="22" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="77"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="77"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="76"/>
+      <c r="S22" s="77"/>
+      <c r="X22" s="75"/>
+      <c r="Y22" s="76"/>
+      <c r="Z22" s="77"/>
+    </row>
+    <row r="23" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="19"/>
+      <c r="E23" s="77"/>
+      <c r="I23" s="19"/>
+      <c r="K23" s="77"/>
+      <c r="Q23" s="19"/>
+      <c r="S23" s="77"/>
+      <c r="X23" s="19"/>
+      <c r="Z23" s="77"/>
+    </row>
+    <row r="24" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="19"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="77"/>
+      <c r="I24" s="19"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="77"/>
+      <c r="Q24" s="19"/>
+      <c r="S24" s="76"/>
+      <c r="T24" s="77"/>
+      <c r="X24" s="19"/>
+      <c r="Z24" s="76"/>
+      <c r="AA24" s="77"/>
+    </row>
+    <row r="25" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="74"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="I25" s="74"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="77"/>
+      <c r="Q25" s="74"/>
+      <c r="S25" s="77"/>
+      <c r="T25" s="77"/>
+      <c r="X25" s="74"/>
+      <c r="Z25" s="77"/>
+      <c r="AA25" s="77"/>
+    </row>
+    <row r="26" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="75"/>
+      <c r="D26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="76"/>
+      <c r="L26" s="77"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="76"/>
+      <c r="T26" s="77"/>
+      <c r="X26" s="75"/>
+      <c r="Y26" s="76"/>
+      <c r="AA26" s="77"/>
+    </row>
+    <row r="27" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="19"/>
+      <c r="F27" s="77"/>
+      <c r="I27" s="19"/>
+      <c r="L27" s="77"/>
+      <c r="Q27" s="19"/>
+      <c r="T27" s="77"/>
+      <c r="X27" s="19"/>
+      <c r="AA27" s="77"/>
+    </row>
+    <row r="28" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="19"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="77"/>
+      <c r="I28" s="19"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="77"/>
+      <c r="Q28" s="19"/>
+      <c r="T28" s="76"/>
+      <c r="U28" s="77"/>
+      <c r="X28" s="19"/>
+      <c r="AA28" s="76"/>
+      <c r="AB28" s="77"/>
+    </row>
+    <row r="29" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="74"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="I29" s="74"/>
+      <c r="L29" s="77"/>
+      <c r="M29" s="77"/>
+      <c r="Q29" s="74"/>
+      <c r="T29" s="77"/>
+      <c r="U29" s="77"/>
+      <c r="X29" s="74"/>
+      <c r="AA29" s="77"/>
+      <c r="AB29" s="77"/>
+    </row>
+    <row r="30" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="75"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="76"/>
+      <c r="S30" s="77"/>
+      <c r="T30" s="77"/>
+      <c r="U30" s="77"/>
+      <c r="X30" s="75"/>
+      <c r="Y30" s="76"/>
+      <c r="Z30" s="77"/>
+      <c r="AA30" s="77"/>
+      <c r="AB30" s="77"/>
+    </row>
+    <row r="31" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="19"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="I31" s="19"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="Q31" s="19"/>
+      <c r="S31" s="77"/>
+      <c r="T31" s="77"/>
+      <c r="U31" s="77"/>
+      <c r="X31" s="19"/>
+      <c r="Z31" s="77"/>
+      <c r="AA31" s="77"/>
+      <c r="AB31" s="77"/>
+    </row>
+    <row r="32" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="19"/>
+      <c r="E32" s="76"/>
+      <c r="G32" s="77"/>
+      <c r="I32" s="19"/>
+      <c r="K32" s="76"/>
+      <c r="M32" s="77"/>
+      <c r="Q32" s="19"/>
+      <c r="S32" s="76"/>
+      <c r="U32" s="77"/>
+      <c r="X32" s="19"/>
+      <c r="Z32" s="76"/>
+      <c r="AB32" s="77"/>
+    </row>
+    <row r="33" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="74"/>
+      <c r="E33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="I33" s="74"/>
+      <c r="K33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="Q33" s="74"/>
+      <c r="S33" s="77"/>
+      <c r="U33" s="77"/>
+      <c r="X33" s="74"/>
+      <c r="Z33" s="77"/>
+      <c r="AB33" s="77"/>
+    </row>
+    <row r="34" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="75"/>
+      <c r="D34" s="76"/>
+      <c r="G34" s="77"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="76"/>
+      <c r="M34" s="77"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="76"/>
+      <c r="U34" s="77"/>
+      <c r="X34" s="75"/>
+      <c r="Y34" s="76"/>
+      <c r="AB34" s="77"/>
+    </row>
+    <row r="35" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G35" s="79">
+        <v>4</v>
+      </c>
+      <c r="M35" s="79">
+        <v>4</v>
+      </c>
+      <c r="U35" s="79">
+        <v>4</v>
+      </c>
+      <c r="AB35" s="79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="19"/>
+      <c r="G36" s="76">
+        <v>3</v>
+      </c>
+      <c r="I36" s="19"/>
+      <c r="M36" s="76">
+        <v>3</v>
+      </c>
+      <c r="Q36" s="19"/>
+      <c r="U36" s="76">
+        <v>3</v>
+      </c>
+      <c r="X36" s="19"/>
+      <c r="AB36" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="74"/>
+      <c r="G37" s="78"/>
+      <c r="I37" s="74"/>
+      <c r="M37" s="78"/>
+      <c r="Q37" s="74"/>
+      <c r="U37" s="78"/>
+      <c r="X37" s="74"/>
+      <c r="AB37" s="78"/>
+    </row>
+    <row r="38" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="75"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="77"/>
+      <c r="G38" s="78"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
+      <c r="M38" s="78"/>
+      <c r="Q38" s="75"/>
+      <c r="R38" s="76"/>
+      <c r="S38" s="77"/>
+      <c r="U38" s="78"/>
+      <c r="X38" s="75"/>
+      <c r="Y38" s="76"/>
+      <c r="Z38" s="77"/>
+      <c r="AB38" s="78"/>
+    </row>
+    <row r="39" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="19"/>
+      <c r="E39" s="77"/>
+      <c r="G39" s="78"/>
+      <c r="I39" s="19"/>
+      <c r="K39" s="77"/>
+      <c r="M39" s="78"/>
+      <c r="Q39" s="19"/>
+      <c r="S39" s="77"/>
+      <c r="U39" s="78"/>
+      <c r="X39" s="19"/>
+      <c r="Z39" s="77"/>
+      <c r="AB39" s="78"/>
+    </row>
+    <row r="40" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="19"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="78"/>
+      <c r="I40" s="19"/>
+      <c r="K40" s="76"/>
+      <c r="L40" s="77"/>
+      <c r="M40" s="78"/>
+      <c r="Q40" s="19"/>
+      <c r="S40" s="76"/>
+      <c r="T40" s="77"/>
+      <c r="U40" s="78"/>
+      <c r="X40" s="19"/>
+      <c r="Z40" s="76"/>
+      <c r="AA40" s="77"/>
+      <c r="AB40" s="78"/>
+    </row>
+    <row r="41" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="74"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="78"/>
+      <c r="I41" s="74"/>
+      <c r="K41" s="77"/>
+      <c r="L41" s="77"/>
+      <c r="M41" s="78"/>
+      <c r="Q41" s="74"/>
+      <c r="S41" s="77"/>
+      <c r="T41" s="77"/>
+      <c r="U41" s="78"/>
+      <c r="X41" s="74"/>
+      <c r="Z41" s="77"/>
+      <c r="AA41" s="77"/>
+      <c r="AB41" s="78"/>
+    </row>
+    <row r="42" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="75"/>
+      <c r="D42" s="76"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="77"/>
+      <c r="I42" s="75"/>
+      <c r="J42" s="76"/>
+      <c r="L42" s="77"/>
+      <c r="M42" s="77"/>
+      <c r="Q42" s="75"/>
+      <c r="R42" s="76"/>
+      <c r="T42" s="77"/>
+      <c r="U42" s="77"/>
+      <c r="X42" s="75"/>
+      <c r="Y42" s="76"/>
+      <c r="AA42" s="77"/>
+      <c r="AB42" s="77"/>
+    </row>
+    <row r="43" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="19"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="I43" s="19"/>
+      <c r="L43" s="77"/>
+      <c r="M43" s="77"/>
+      <c r="Q43" s="19"/>
+      <c r="T43" s="77"/>
+      <c r="U43" s="77"/>
+      <c r="X43" s="19"/>
+      <c r="AA43" s="77"/>
+      <c r="AB43" s="77"/>
+    </row>
+    <row r="44" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="19"/>
+      <c r="F44" s="76"/>
+      <c r="I44" s="19"/>
+      <c r="L44" s="76"/>
+      <c r="Q44" s="19"/>
+      <c r="T44" s="76"/>
+      <c r="X44" s="19"/>
+      <c r="AA44" s="76"/>
+    </row>
+    <row r="45" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C45" s="74"/>
+      <c r="F45" s="77"/>
+      <c r="I45" s="74"/>
+      <c r="L45" s="77"/>
+      <c r="Q45" s="74"/>
+      <c r="T45" s="77"/>
+      <c r="X45" s="74"/>
+      <c r="AA45" s="77"/>
+    </row>
+    <row r="46" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C46" s="75"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="77"/>
+      <c r="I46" s="75"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="77"/>
+      <c r="Q46" s="75"/>
+      <c r="R46" s="76"/>
+      <c r="S46" s="77"/>
+      <c r="T46" s="77"/>
+      <c r="X46" s="75"/>
+      <c r="Y46" s="76"/>
+      <c r="Z46" s="77"/>
+      <c r="AA46" s="77"/>
+    </row>
+    <row r="47" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C47" s="19"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="77"/>
+      <c r="I47" s="19"/>
+      <c r="K47" s="77"/>
+      <c r="L47" s="77"/>
+      <c r="Q47" s="19"/>
+      <c r="S47" s="77"/>
+      <c r="T47" s="77"/>
+      <c r="X47" s="19"/>
+      <c r="Z47" s="77"/>
+      <c r="AA47" s="77"/>
+    </row>
+    <row r="48" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C48" s="19"/>
+      <c r="E48" s="76"/>
+      <c r="I48" s="19"/>
+      <c r="K48" s="76"/>
+      <c r="Q48" s="19"/>
+      <c r="S48" s="76"/>
+      <c r="X48" s="19"/>
+      <c r="Z48" s="76"/>
+    </row>
+    <row r="49" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C49" s="74"/>
+      <c r="E49" s="77"/>
+      <c r="I49" s="74"/>
+      <c r="K49" s="77"/>
+      <c r="Q49" s="74"/>
+      <c r="S49" s="77"/>
+      <c r="X49" s="74"/>
+      <c r="Z49" s="77"/>
+    </row>
+    <row r="50" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C50" s="75"/>
+      <c r="D50" s="76"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="76"/>
+      <c r="Q50" s="75"/>
+      <c r="R50" s="76"/>
+      <c r="X50" s="75"/>
+      <c r="Y50" s="76"/>
+    </row>
+    <row r="51" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F52" s="74"/>
+      <c r="G52" s="80">
+        <v>3</v>
+      </c>
+      <c r="L52" s="19"/>
+      <c r="T52" s="74"/>
+      <c r="U52" s="80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F53" s="75"/>
+      <c r="G53" s="76">
+        <v>2</v>
+      </c>
+      <c r="L53" s="74"/>
+      <c r="M53" s="80">
+        <v>3</v>
+      </c>
+      <c r="T53" s="75"/>
+      <c r="U53" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K54" s="74"/>
+      <c r="M54" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E55" s="74"/>
+      <c r="K55" s="75"/>
+      <c r="L55" s="76"/>
+    </row>
+    <row r="56" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E56" s="75"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="77"/>
+      <c r="L56" s="19"/>
+      <c r="S56" s="19"/>
+      <c r="Z56" s="19"/>
+      <c r="AA56" s="74"/>
+      <c r="AB56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E57" s="19"/>
+      <c r="G57" s="77">
+        <v>3</v>
+      </c>
+      <c r="L57" s="74"/>
+      <c r="M57">
+        <v>3</v>
+      </c>
+      <c r="S57" s="74"/>
+      <c r="Z57" s="74"/>
+      <c r="AB57" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E58" s="19"/>
+      <c r="G58" s="76">
+        <v>2</v>
+      </c>
+      <c r="K58" s="74"/>
+      <c r="M58" s="76">
+        <v>2</v>
+      </c>
+      <c r="R58" s="74"/>
+      <c r="T58" s="76"/>
+      <c r="U58" s="77"/>
+      <c r="Y58" s="74"/>
+      <c r="AA58" s="76"/>
+    </row>
+    <row r="59" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E59" s="74"/>
+      <c r="G59" s="77"/>
+      <c r="K59" s="75"/>
+      <c r="L59" s="76"/>
+      <c r="R59" s="75"/>
+      <c r="S59" s="76"/>
+      <c r="U59" s="77">
+        <v>3</v>
+      </c>
+      <c r="Y59" s="75"/>
+      <c r="Z59" s="76"/>
+    </row>
+    <row r="60" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E60" s="75"/>
+      <c r="F60" s="76"/>
+      <c r="S60" s="19"/>
+      <c r="U60" s="76">
+        <v>2</v>
+      </c>
+      <c r="Z60" s="19"/>
+      <c r="AA60" s="74"/>
+      <c r="AB60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S61" s="74"/>
+      <c r="U61" s="77"/>
+      <c r="Z61" s="74"/>
+      <c r="AB61" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F62" s="74"/>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="L62" s="74"/>
+      <c r="M62" s="80">
+        <v>2</v>
+      </c>
+      <c r="R62" s="74"/>
+      <c r="T62" s="76"/>
+      <c r="Y62" s="74"/>
+      <c r="AA62" s="76"/>
+    </row>
+    <row r="63" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F63" s="75"/>
+      <c r="G63" s="76">
+        <v>1</v>
+      </c>
+      <c r="L63" s="75"/>
+      <c r="M63" s="76">
+        <v>1</v>
+      </c>
+      <c r="R63" s="75"/>
+      <c r="S63" s="76"/>
+      <c r="Y63" s="75"/>
+      <c r="Z63" s="76"/>
+    </row>
+    <row r="64" spans="3:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S64" s="19"/>
+      <c r="Z64" s="19"/>
+    </row>
+    <row r="65" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S65" s="74"/>
+      <c r="Z65" s="74"/>
+    </row>
+    <row r="66" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="R66" s="74"/>
+      <c r="T66" s="76"/>
+      <c r="U66" s="77"/>
+      <c r="Y66" s="74"/>
+      <c r="AA66" s="76"/>
+      <c r="AB66" s="77"/>
+    </row>
+    <row r="67" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D67" s="74"/>
+      <c r="J67" s="74"/>
+      <c r="R67" s="75"/>
+      <c r="S67" s="76"/>
+      <c r="U67" s="77">
+        <v>3</v>
+      </c>
+      <c r="Y67" s="75"/>
+      <c r="Z67" s="76"/>
+      <c r="AB67" s="77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D68" s="75"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="77"/>
+      <c r="J68" s="75"/>
+      <c r="K68" s="76"/>
+      <c r="L68" s="77"/>
+      <c r="S68" s="19"/>
+      <c r="U68" s="76">
+        <v>2</v>
+      </c>
+      <c r="Z68" s="19"/>
+      <c r="AB68" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D69" s="19"/>
+      <c r="F69" s="77"/>
+      <c r="J69" s="19"/>
+      <c r="L69" s="77"/>
+      <c r="S69" s="74"/>
+      <c r="U69" s="77"/>
+      <c r="Z69" s="74"/>
+      <c r="AB69" s="77"/>
+    </row>
+    <row r="70" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D70" s="19"/>
+      <c r="F70" s="76"/>
+      <c r="G70" s="77"/>
+      <c r="J70" s="19"/>
+      <c r="L70" s="76"/>
+      <c r="M70" s="77"/>
+      <c r="R70" s="74"/>
+      <c r="T70" s="76"/>
+      <c r="Y70" s="74"/>
+      <c r="AA70" s="76"/>
+    </row>
+    <row r="71" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D71" s="74"/>
+      <c r="F71" s="77"/>
+      <c r="G71" s="77"/>
+      <c r="J71" s="74"/>
+      <c r="L71" s="77"/>
+      <c r="M71" s="77"/>
+      <c r="R71" s="75"/>
+      <c r="S71" s="76"/>
+      <c r="Y71" s="75"/>
+      <c r="Z71" s="76"/>
+    </row>
+    <row r="72" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D72" s="75"/>
+      <c r="E72" s="76"/>
+      <c r="G72" s="77"/>
+      <c r="J72" s="75"/>
+      <c r="K72" s="76"/>
+      <c r="M72" s="77"/>
+      <c r="T72" s="74"/>
+      <c r="U72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D73" s="19"/>
+      <c r="G73" s="77">
+        <v>3</v>
+      </c>
+      <c r="J73" s="19"/>
+      <c r="M73" s="77">
+        <v>3</v>
+      </c>
+      <c r="T73" s="75"/>
+      <c r="U73" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D74" s="19"/>
+      <c r="G74" s="76">
+        <v>2</v>
+      </c>
+      <c r="J74" s="19"/>
+      <c r="M74" s="76">
+        <v>2</v>
+      </c>
+      <c r="AA74" s="74"/>
+      <c r="AB74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D75" s="74"/>
+      <c r="G75" s="77"/>
+      <c r="J75" s="74"/>
+      <c r="M75" s="77"/>
+      <c r="T75" s="74"/>
+      <c r="U75">
+        <v>2</v>
+      </c>
+      <c r="AA75" s="75"/>
+      <c r="AB75" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D76" s="75"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="77"/>
+      <c r="G76" s="77"/>
+      <c r="J76" s="75"/>
+      <c r="K76" s="76"/>
+      <c r="L76" s="77"/>
+      <c r="M76" s="77"/>
+      <c r="T76" s="75"/>
+      <c r="U76" s="76">
+        <v>1</v>
+      </c>
+      <c r="AA76" s="19"/>
+    </row>
+    <row r="77" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D77" s="19"/>
+      <c r="F77" s="77"/>
+      <c r="G77" s="77"/>
+      <c r="J77" s="19"/>
+      <c r="L77" s="77"/>
+      <c r="M77" s="77"/>
+      <c r="AA77" s="74"/>
+      <c r="AB77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D78" s="19"/>
+      <c r="F78" s="76"/>
+      <c r="J78" s="19"/>
+      <c r="L78" s="76"/>
+      <c r="S78" s="74"/>
+      <c r="Z78" s="74"/>
+      <c r="AA78" s="75"/>
+      <c r="AB78" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D79" s="74"/>
+      <c r="F79" s="77"/>
+      <c r="J79" s="74"/>
+      <c r="L79" s="77"/>
+      <c r="S79" s="75"/>
+      <c r="T79" s="76"/>
+      <c r="U79" s="77"/>
+      <c r="Z79" s="75"/>
+      <c r="AA79" s="76"/>
+    </row>
+    <row r="80" spans="4:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D80" s="75"/>
+      <c r="E80" s="76"/>
+      <c r="J80" s="75"/>
+      <c r="K80" s="76"/>
+      <c r="S80" s="19"/>
+      <c r="U80" s="77">
+        <v>2</v>
+      </c>
+      <c r="Z80" s="19"/>
+    </row>
+    <row r="81" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S81" s="19"/>
+      <c r="U81" s="76">
+        <v>1</v>
+      </c>
+      <c r="Z81" s="19"/>
+      <c r="AA81" s="74"/>
+      <c r="AB81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F82" s="74"/>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="L82" s="19"/>
+      <c r="S82" s="74"/>
+      <c r="U82" s="77"/>
+      <c r="Z82" s="74"/>
+      <c r="AA82" s="75"/>
+      <c r="AB82" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F83" s="75"/>
+      <c r="G83" s="76">
+        <v>1</v>
+      </c>
+      <c r="L83" s="74"/>
+      <c r="M83" s="80">
+        <v>2</v>
+      </c>
+      <c r="S83" s="75"/>
+      <c r="T83" s="76"/>
+      <c r="Z83" s="75"/>
+      <c r="AA83" s="76"/>
+    </row>
+    <row r="84" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K84" s="74"/>
+      <c r="M84" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E85" s="74"/>
+      <c r="K85" s="75"/>
+      <c r="L85" s="76"/>
+      <c r="T85" s="74"/>
+      <c r="U85">
+        <v>1</v>
+      </c>
+      <c r="AA85" s="74"/>
+      <c r="AB85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E86" s="75"/>
+      <c r="F86" s="76"/>
+      <c r="G86" s="77"/>
+      <c r="L86" s="19"/>
+      <c r="T86" s="75"/>
+      <c r="U86" s="76">
+        <v>0</v>
+      </c>
+      <c r="AA86" s="75"/>
+      <c r="AB86" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E87" s="19"/>
+      <c r="G87" s="79">
+        <v>2</v>
+      </c>
+      <c r="L87" s="74"/>
+      <c r="M87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E88" s="19"/>
+      <c r="G88" s="76">
+        <v>1</v>
+      </c>
+      <c r="K88" s="74"/>
+      <c r="M88" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E89" s="74"/>
+      <c r="G89" s="77"/>
+      <c r="K89" s="75"/>
+      <c r="L89" s="76"/>
+    </row>
+    <row r="90" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E90" s="75"/>
+      <c r="F90" s="76"/>
+    </row>
+    <row r="91" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F92" s="74"/>
+      <c r="G92" s="80">
+        <v>1</v>
+      </c>
+      <c r="L92" s="74"/>
+      <c r="M92" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="5:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F93" s="75"/>
+      <c r="G93" s="76">
+        <v>0</v>
+      </c>
+      <c r="L93" s="75"/>
+      <c r="M93" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="5:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <conditionalFormatting sqref="A3:A18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12329,7 +13460,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="74"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -12337,7 +13468,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="74"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
@@ -12371,7 +13502,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="74"/>
+      <c r="D12" s="81"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -12379,7 +13510,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="74"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
@@ -12413,7 +13544,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="74"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -12421,7 +13552,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="74"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -12517,7 +13648,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="74"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -12527,7 +13658,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="74"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -12537,32 +13668,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="84" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="80"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="87"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="77"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="80"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="87"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="78"/>
+      <c r="B12" s="85"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="80"/>
+      <c r="E12" s="87"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -12570,37 +13701,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="84" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="80"/>
+      <c r="E13" s="87"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="75" t="s">
+      <c r="I13" s="82" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="79"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="86"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="75"/>
+      <c r="I14" s="82"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="79"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="86"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="76"/>
+      <c r="I15" s="83"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -12609,7 +13740,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="74"/>
+      <c r="F16" s="81"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -12619,7 +13750,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="74"/>
+      <c r="F17" s="81"/>
       <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
@@ -12657,9 +13788,9 @@
         <v>27</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -12667,9 +13798,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Working on multibracket considerations and standard multibrackets
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6971372-E574-421E-8517-20E75F8344E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796EB346-D7C6-4E7F-A8B8-B5F4CBF030C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="21" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="19" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="131">
   <si>
     <t>Georgia</t>
   </si>
@@ -444,6 +444,12 @@
   </si>
   <si>
     <t>Grizzlies</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
 </sst>
 </file>
@@ -910,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1039,10 +1045,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1051,10 +1054,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,6 +1068,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3269,7 +3285,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="83" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3278,7 +3294,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="85"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3324,7 +3340,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="84" t="s">
+      <c r="D17" s="83" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3333,7 +3349,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="85"/>
+      <c r="D18" s="84"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -3764,7 +3780,7 @@
   <dimension ref="B4:BI28"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="XFD19" sqref="XFD19"/>
+      <selection activeCell="H5" sqref="H5:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6859,7 +6875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D84D55B-86DB-41A7-86B6-8D3E6C4FEE99}">
   <dimension ref="C4:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E14" sqref="E14:H28"/>
     </sheetView>
   </sheetViews>
@@ -7420,15 +7436,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A138887D-E83F-4832-AC66-DEE1E0C0D3AC}">
-  <dimension ref="A4:O33"/>
+  <dimension ref="A4:AC33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="C6:E13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -7444,8 +7460,22 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -7461,8 +7491,42 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P5" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>3</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1">
+        <v>4</v>
+      </c>
+      <c r="X5" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+    </row>
+    <row r="6" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -7480,10 +7544,32 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="90">
+        <v>4</v>
+      </c>
+      <c r="R6" s="1">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="91"/>
+      <c r="Y6" s="90"/>
+      <c r="Z6" s="90"/>
+      <c r="AA6" s="90"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -7501,10 +7587,24 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N7" s="90"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="90"/>
+      <c r="V7" s="90"/>
+      <c r="W7" s="90"/>
+      <c r="X7" s="91"/>
+      <c r="Y7" s="90"/>
+      <c r="Z7" s="90"/>
+      <c r="AA7" s="90"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="7"/>
@@ -7520,10 +7620,24 @@
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="91"/>
+      <c r="X8" s="90"/>
+      <c r="Y8" s="90"/>
+      <c r="Z8" s="90"/>
+      <c r="AA8" s="90"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+    </row>
+    <row r="9" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
@@ -7539,10 +7653,26 @@
       <c r="K9" s="1"/>
       <c r="L9" s="5"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="91"/>
+      <c r="W9" s="90"/>
+      <c r="X9" s="90"/>
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="90"/>
+      <c r="AA9" s="90"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+    </row>
+    <row r="10" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -7562,10 +7692,26 @@
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="90"/>
+      <c r="X10" s="91"/>
+      <c r="Y10" s="90"/>
+      <c r="Z10" s="90"/>
+      <c r="AA10" s="90"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+    </row>
+    <row r="11" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -7583,10 +7729,24 @@
       <c r="K11" s="1"/>
       <c r="L11" s="5"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="90"/>
+      <c r="V11" s="90"/>
+      <c r="W11" s="90"/>
+      <c r="X11" s="91"/>
+      <c r="Y11" s="90"/>
+      <c r="Z11" s="90"/>
+      <c r="AA11" s="90"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>111</v>
@@ -7602,10 +7762,24 @@
       <c r="K12" s="4"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="90"/>
+      <c r="Q12" s="90"/>
+      <c r="R12" s="90"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="90"/>
+      <c r="V12" s="90"/>
+      <c r="W12" s="91"/>
+      <c r="X12" s="90"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="90"/>
+      <c r="AA12" s="90"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="1"/>
@@ -7621,10 +7795,26 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N13" s="90"/>
+      <c r="O13" s="90"/>
+      <c r="P13" s="91"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="T13" s="5"/>
+      <c r="U13" s="90"/>
+      <c r="V13" s="90"/>
+      <c r="W13" s="91"/>
+      <c r="X13" s="90"/>
+      <c r="Y13" s="90"/>
+      <c r="Z13" s="90"/>
+      <c r="AA13" s="90"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
         <v>111</v>
@@ -7640,10 +7830,24 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="90"/>
+      <c r="O14" s="90"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="90"/>
+      <c r="X14" s="90"/>
+      <c r="Y14" s="90"/>
+      <c r="Z14" s="90"/>
+      <c r="AA14" s="90"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -7657,10 +7861,26 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N15" s="90"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="90"/>
+      <c r="V15" s="90"/>
+      <c r="W15" s="90"/>
+      <c r="X15" s="90"/>
+      <c r="Y15" s="90"/>
+      <c r="Z15" s="90"/>
+      <c r="AA15" s="90"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -7674,10 +7894,26 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="90"/>
+      <c r="V16" s="90"/>
+      <c r="W16" s="90"/>
+      <c r="X16" s="90"/>
+      <c r="Y16" s="90"/>
+      <c r="Z16" s="90"/>
+      <c r="AA16" s="90"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+    </row>
+    <row r="17" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -7691,10 +7927,26 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="90"/>
+      <c r="AA17" s="90"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+    </row>
+    <row r="18" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -7708,10 +7960,24 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="90"/>
+      <c r="AA18" s="90"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+    </row>
+    <row r="19" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -7725,10 +7991,26 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N19" s="90"/>
+      <c r="O19" s="90"/>
+      <c r="P19" s="91"/>
+      <c r="Q19" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="90"/>
+      <c r="V19" s="90"/>
+      <c r="W19" s="90"/>
+      <c r="X19" s="90"/>
+      <c r="Y19" s="90"/>
+      <c r="Z19" s="90"/>
+      <c r="AA19" s="90"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+    </row>
+    <row r="20" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -7744,10 +8026,26 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N20" s="90"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="92"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="90"/>
+      <c r="V20" s="90"/>
+      <c r="W20" s="91"/>
+      <c r="X20" s="90"/>
+      <c r="Y20" s="90"/>
+      <c r="Z20" s="90"/>
+      <c r="AA20" s="90"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -7763,10 +8061,24 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N21" s="90"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="90"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="90"/>
+      <c r="V21" s="91"/>
+      <c r="W21" s="91"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="90"/>
+      <c r="Z21" s="90"/>
+      <c r="AA21" s="90"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+    </row>
+    <row r="22" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="6" t="s">
@@ -7784,10 +8096,26 @@
       <c r="K22" s="5"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N22" s="90"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="90"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T22" s="93"/>
+      <c r="U22" s="90"/>
+      <c r="V22" s="91"/>
+      <c r="W22" s="90"/>
+      <c r="X22" s="90"/>
+      <c r="Y22" s="90"/>
+      <c r="Z22" s="90"/>
+      <c r="AA22" s="90"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+    </row>
+    <row r="23" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="7"/>
@@ -7801,10 +8129,26 @@
       <c r="K23" s="5"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N23" s="90"/>
+      <c r="O23" s="90"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="90"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="90"/>
+      <c r="X23" s="90"/>
+      <c r="Y23" s="90"/>
+      <c r="Z23" s="90"/>
+      <c r="AA23" s="90"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+    </row>
+    <row r="24" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8" t="s">
@@ -7822,10 +8166,26 @@
       <c r="K24" s="5"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N24" s="90"/>
+      <c r="O24" s="90"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="91"/>
+      <c r="R24" s="90"/>
+      <c r="S24" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="T24" s="4"/>
+      <c r="U24" s="90"/>
+      <c r="V24" s="91"/>
+      <c r="W24" s="91"/>
+      <c r="X24" s="90"/>
+      <c r="Y24" s="90"/>
+      <c r="Z24" s="90"/>
+      <c r="AA24" s="90"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+    </row>
+    <row r="25" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -7841,10 +8201,24 @@
       <c r="K25" s="4"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="91"/>
+      <c r="S25" s="90"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="91"/>
+      <c r="W25" s="90"/>
+      <c r="X25" s="90"/>
+      <c r="Y25" s="90"/>
+      <c r="Z25" s="90"/>
+      <c r="AA25" s="90"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+    </row>
+    <row r="26" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="6" t="s">
@@ -7862,10 +8236,24 @@
       <c r="K26" s="5"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N26" s="90"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="90"/>
+      <c r="Q26" s="91"/>
+      <c r="R26" s="91"/>
+      <c r="S26" s="90"/>
+      <c r="T26" s="90"/>
+      <c r="U26" s="90"/>
+      <c r="V26" s="91"/>
+      <c r="W26" s="90"/>
+      <c r="X26" s="90"/>
+      <c r="Y26" s="90"/>
+      <c r="Z26" s="90"/>
+      <c r="AA26" s="90"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+    </row>
+    <row r="27" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="7"/>
@@ -7879,10 +8267,24 @@
       <c r="K27" s="5"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="90"/>
+      <c r="Q27" s="91"/>
+      <c r="R27" s="90"/>
+      <c r="S27" s="90"/>
+      <c r="T27" s="90"/>
+      <c r="U27" s="90"/>
+      <c r="V27" s="90"/>
+      <c r="W27" s="90"/>
+      <c r="X27" s="90"/>
+      <c r="Y27" s="90"/>
+      <c r="Z27" s="90"/>
+      <c r="AA27" s="90"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+    </row>
+    <row r="28" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
@@ -7900,10 +8302,24 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="90"/>
+      <c r="Q28" s="91"/>
+      <c r="R28" s="90"/>
+      <c r="S28" s="90"/>
+      <c r="T28" s="90"/>
+      <c r="U28" s="90"/>
+      <c r="V28" s="91"/>
+      <c r="W28" s="90"/>
+      <c r="X28" s="90"/>
+      <c r="Y28" s="90"/>
+      <c r="Z28" s="90"/>
+      <c r="AA28" s="90"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+    </row>
+    <row r="29" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -7917,10 +8333,24 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="90"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="90"/>
+      <c r="S29" s="90"/>
+      <c r="T29" s="90"/>
+      <c r="U29" s="90"/>
+      <c r="V29" s="91"/>
+      <c r="W29" s="90"/>
+      <c r="X29" s="90"/>
+      <c r="Y29" s="90"/>
+      <c r="Z29" s="90"/>
+      <c r="AA29" s="90"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+    </row>
+    <row r="30" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -7936,10 +8366,24 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="90"/>
+      <c r="R30" s="90"/>
+      <c r="S30" s="90"/>
+      <c r="T30" s="90"/>
+      <c r="U30" s="90"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="90"/>
+      <c r="X30" s="90"/>
+      <c r="Y30" s="90"/>
+      <c r="Z30" s="90"/>
+      <c r="AA30" s="90"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+    </row>
+    <row r="31" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -7953,10 +8397,24 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N31" s="90"/>
+      <c r="O31" s="90"/>
+      <c r="P31" s="90"/>
+      <c r="Q31" s="90"/>
+      <c r="R31" s="90"/>
+      <c r="S31" s="90"/>
+      <c r="T31" s="90"/>
+      <c r="U31" s="90"/>
+      <c r="V31" s="90"/>
+      <c r="W31" s="90"/>
+      <c r="X31" s="90"/>
+      <c r="Y31" s="90"/>
+      <c r="Z31" s="90"/>
+      <c r="AA31" s="90"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -7970,10 +8428,24 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N32" s="90"/>
+      <c r="O32" s="90"/>
+      <c r="P32" s="90"/>
+      <c r="Q32" s="90"/>
+      <c r="R32" s="90"/>
+      <c r="S32" s="90"/>
+      <c r="T32" s="90"/>
+      <c r="U32" s="90"/>
+      <c r="V32" s="90"/>
+      <c r="W32" s="90"/>
+      <c r="X32" s="90"/>
+      <c r="Y32" s="90"/>
+      <c r="Z32" s="90"/>
+      <c r="AA32" s="90"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -7987,8 +8459,22 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="N33" s="90"/>
+      <c r="O33" s="90"/>
+      <c r="P33" s="90"/>
+      <c r="Q33" s="90"/>
+      <c r="R33" s="90"/>
+      <c r="S33" s="90"/>
+      <c r="T33" s="90"/>
+      <c r="U33" s="90"/>
+      <c r="V33" s="90"/>
+      <c r="W33" s="90"/>
+      <c r="X33" s="90"/>
+      <c r="Y33" s="90"/>
+      <c r="Z33" s="90"/>
+      <c r="AA33" s="90"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8587,7 +9073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FC37AD-F8C8-422A-907B-37F83257262D}">
   <dimension ref="A3:AB94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AC71" sqref="Z71:AC83"/>
     </sheetView>
@@ -13668,32 +14154,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="83" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="82"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="84"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="82"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="85"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="87"/>
+      <c r="E12" s="82"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -13701,37 +14187,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="83" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="87"/>
+      <c r="E13" s="82"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="82" t="s">
+      <c r="I13" s="85" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="86"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="82"/>
+      <c r="I14" s="85"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="86"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="87"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="83"/>
+      <c r="I15" s="86"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -13819,17 +14305,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to weakly proper definition and swiss proofs
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796EB346-D7C6-4E7F-A8B8-B5F4CBF030C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8B1185-7C86-45A4-AC67-6F462D7F92A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="19" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="22" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="Sheet19" sheetId="21" r:id="rId20"/>
     <sheet name="Sheet20" sheetId="22" r:id="rId21"/>
     <sheet name="Sheet21" sheetId="23" r:id="rId22"/>
+    <sheet name="Sheet22" sheetId="24" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="131">
   <si>
     <t>Georgia</t>
   </si>
@@ -3105,7 +3106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AADE0C-132A-4EF3-A172-B6CF6F69AB44}">
   <dimension ref="B7:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -3777,10 +3778,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
-  <dimension ref="B4:BI28"/>
+  <dimension ref="B4:BO28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:K22"/>
+    <sheetView topLeftCell="Y4" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5:AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3791,7 +3792,7 @@
     <col min="9" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:61" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:67" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3852,8 +3853,14 @@
       <c r="BG4" s="1"/>
       <c r="BH4" s="1"/>
       <c r="BI4" s="1"/>
-    </row>
-    <row r="5" spans="2:61" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ4" s="1"/>
+      <c r="BK4" s="1"/>
+      <c r="BL4" s="1"/>
+      <c r="BM4" s="1"/>
+      <c r="BN4" s="1"/>
+      <c r="BO4" s="1"/>
+    </row>
+    <row r="5" spans="2:67" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="C5" s="6">
         <v>1</v>
@@ -3916,26 +3923,34 @@
       <c r="AS5" s="1"/>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
-      <c r="AV5" s="1"/>
-      <c r="AW5" s="6">
-        <v>1</v>
-      </c>
+      <c r="AV5" s="6">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
       <c r="BA5" s="1"/>
       <c r="BB5" s="1"/>
-      <c r="BC5" s="1"/>
-      <c r="BD5" s="6">
-        <v>1</v>
-      </c>
+      <c r="BC5" s="6">
+        <v>1</v>
+      </c>
+      <c r="BD5" s="1"/>
       <c r="BE5" s="1"/>
       <c r="BF5" s="1"/>
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
-    </row>
-    <row r="6" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ5" s="6">
+        <v>1</v>
+      </c>
+      <c r="BK5" s="1"/>
+      <c r="BL5" s="1"/>
+      <c r="BM5" s="1"/>
+      <c r="BN5" s="1"/>
+      <c r="BO5" s="1"/>
+    </row>
+    <row r="6" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="66" t="s">
         <v>59</v>
@@ -3977,7 +3992,9 @@
       <c r="AD6" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="AE6" s="1"/>
+      <c r="AE6" s="6">
+        <v>1</v>
+      </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
@@ -3998,26 +4015,34 @@
       <c r="AS6" s="1"/>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="66" t="s">
+      <c r="AV6" s="66" t="s">
         <v>59</v>
       </c>
+      <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
       <c r="AY6" s="1"/>
       <c r="AZ6" s="1"/>
       <c r="BA6" s="1"/>
       <c r="BB6" s="1"/>
-      <c r="BC6" s="1"/>
-      <c r="BD6" s="66" t="s">
+      <c r="BC6" s="66" t="s">
         <v>59</v>
       </c>
+      <c r="BD6" s="1"/>
       <c r="BE6" s="1"/>
       <c r="BF6" s="1"/>
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
       <c r="BI6" s="1"/>
-    </row>
-    <row r="7" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ6" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK6" s="1"/>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+    </row>
+    <row r="7" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="8">
         <v>8</v>
@@ -4080,26 +4105,34 @@
       <c r="AS7" s="1"/>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
-      <c r="AV7" s="1"/>
-      <c r="AW7" s="8">
+      <c r="AV7" s="8">
         <v>8</v>
       </c>
-      <c r="AX7" s="4"/>
-      <c r="AY7" s="5"/>
+      <c r="AW7" s="4"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
-      <c r="BC7" s="1"/>
-      <c r="BD7" s="8">
+      <c r="BC7" s="8">
         <v>8</v>
       </c>
-      <c r="BE7" s="4"/>
-      <c r="BF7" s="5"/>
+      <c r="BD7" s="4"/>
+      <c r="BE7" s="5"/>
+      <c r="BF7" s="1"/>
       <c r="BG7" s="1"/>
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
-    </row>
-    <row r="8" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ7" s="8">
+        <v>8</v>
+      </c>
+      <c r="BK7" s="4"/>
+      <c r="BL7" s="5"/>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+    </row>
+    <row r="8" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="6"/>
       <c r="D8" s="59" t="s">
@@ -4142,7 +4175,9 @@
       <c r="AE8" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="AF8" s="5"/>
+      <c r="AF8" s="21">
+        <v>1</v>
+      </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
@@ -4162,26 +4197,34 @@
       <c r="AS8" s="1"/>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
-      <c r="AV8" s="1"/>
-      <c r="AW8" s="6"/>
-      <c r="AX8" s="59" t="s">
+      <c r="AV8" s="6"/>
+      <c r="AW8" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="AY8" s="5"/>
+      <c r="AX8" s="5"/>
+      <c r="AY8" s="1"/>
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
       <c r="BB8" s="1"/>
-      <c r="BC8" s="1"/>
-      <c r="BD8" s="6"/>
-      <c r="BE8" s="59" t="s">
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="BF8" s="5"/>
+      <c r="BE8" s="5"/>
+      <c r="BF8" s="1"/>
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
       <c r="BI8" s="1"/>
-    </row>
-    <row r="9" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ8" s="6"/>
+      <c r="BK8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL8" s="5"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+    </row>
+    <row r="9" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="6">
         <v>4</v>
@@ -4244,26 +4287,34 @@
       <c r="AS9" s="5"/>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-      <c r="AW9" s="6">
+      <c r="AV9" s="6">
         <v>4</v>
       </c>
-      <c r="AX9" s="1"/>
-      <c r="AY9" s="4"/>
-      <c r="AZ9" s="5"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="4"/>
+      <c r="AY9" s="5"/>
+      <c r="AZ9" s="1"/>
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
-      <c r="BC9" s="1"/>
-      <c r="BD9" s="6">
+      <c r="BC9" s="6">
         <v>4</v>
       </c>
-      <c r="BE9" s="1"/>
-      <c r="BF9" s="4"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="4"/>
+      <c r="BF9" s="5"/>
       <c r="BG9" s="1"/>
       <c r="BH9" s="1"/>
       <c r="BI9" s="1"/>
-    </row>
-    <row r="10" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ9" s="6">
+        <v>4</v>
+      </c>
+      <c r="BK9" s="1"/>
+      <c r="BL9" s="4"/>
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+      <c r="BO9" s="1"/>
+    </row>
+    <row r="10" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="66" t="s">
         <v>60</v>
@@ -4305,7 +4356,9 @@
       <c r="AD10" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="AE10" s="1"/>
+      <c r="AE10" s="6">
+        <v>4</v>
+      </c>
       <c r="AF10" s="5"/>
       <c r="AG10" s="5"/>
       <c r="AH10" s="1"/>
@@ -4326,26 +4379,34 @@
       <c r="AS10" s="5"/>
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="66" t="s">
+      <c r="AV10" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="AX10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="5"/>
       <c r="AY10" s="5"/>
-      <c r="AZ10" s="5"/>
+      <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
       <c r="BB10" s="1"/>
-      <c r="BC10" s="1"/>
-      <c r="BD10" s="66" t="s">
+      <c r="BC10" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="BE10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="5"/>
       <c r="BF10" s="5"/>
       <c r="BG10" s="1"/>
       <c r="BH10" s="1"/>
       <c r="BI10" s="1"/>
-    </row>
-    <row r="11" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ10" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK10" s="1"/>
+      <c r="BL10" s="5"/>
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+    </row>
+    <row r="11" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="8">
         <v>5</v>
@@ -4408,26 +4469,34 @@
       <c r="AS11" s="5"/>
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
-      <c r="AV11" s="1"/>
-      <c r="AW11" s="8">
+      <c r="AV11" s="8">
         <v>5</v>
       </c>
-      <c r="AX11" s="4"/>
-      <c r="AY11" s="1"/>
-      <c r="AZ11" s="5"/>
+      <c r="AW11" s="4"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="5"/>
+      <c r="AZ11" s="1"/>
       <c r="BA11" s="1"/>
       <c r="BB11" s="1"/>
-      <c r="BC11" s="1"/>
-      <c r="BD11" s="8">
+      <c r="BC11" s="8">
         <v>5</v>
       </c>
-      <c r="BE11" s="4"/>
-      <c r="BF11" s="1"/>
+      <c r="BD11" s="4"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="5"/>
       <c r="BG11" s="1"/>
       <c r="BH11" s="1"/>
       <c r="BI11" s="1"/>
-    </row>
-    <row r="12" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ11" s="8">
+        <v>5</v>
+      </c>
+      <c r="BK11" s="4"/>
+      <c r="BL11" s="1"/>
+      <c r="BM11" s="1"/>
+      <c r="BN11" s="1"/>
+      <c r="BO11" s="1"/>
+    </row>
+    <row r="12" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
@@ -4471,7 +4540,9 @@
       <c r="AF12" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="AG12" s="5"/>
+      <c r="AG12" s="21">
+        <v>1</v>
+      </c>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="6"/>
@@ -4490,24 +4561,32 @@
       <c r="AS12" s="5"/>
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
-      <c r="AV12" s="1"/>
-      <c r="AW12" s="6"/>
-      <c r="AX12" s="1"/>
-      <c r="AY12" s="59" t="s">
+      <c r="AV12" s="6"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="AZ12" s="5"/>
+      <c r="AY12" s="5"/>
+      <c r="AZ12" s="1"/>
       <c r="BA12" s="1"/>
       <c r="BB12" s="1"/>
-      <c r="BC12" s="1"/>
-      <c r="BD12" s="6"/>
-      <c r="BE12" s="1"/>
-      <c r="BF12" s="59"/>
+      <c r="BC12" s="6"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="BF12" s="5"/>
       <c r="BG12" s="1"/>
       <c r="BH12" s="1"/>
       <c r="BI12" s="1"/>
-    </row>
-    <row r="13" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ12" s="6"/>
+      <c r="BK12" s="1"/>
+      <c r="BL12" s="59"/>
+      <c r="BM12" s="1"/>
+      <c r="BN12" s="1"/>
+      <c r="BO12" s="1"/>
+    </row>
+    <row r="13" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="6">
         <v>3</v>
@@ -4570,26 +4649,34 @@
       <c r="AS13" s="4"/>
       <c r="AT13" s="1"/>
       <c r="AU13" s="1"/>
-      <c r="AV13" s="1"/>
-      <c r="AW13" s="6">
+      <c r="AV13" s="6">
         <v>3</v>
       </c>
+      <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
-      <c r="AY13" s="1"/>
-      <c r="AZ13" s="4"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
       <c r="BB13" s="1"/>
-      <c r="BC13" s="1"/>
-      <c r="BD13" s="6">
+      <c r="BC13" s="6">
         <v>3</v>
       </c>
+      <c r="BD13" s="1"/>
       <c r="BE13" s="1"/>
-      <c r="BF13" s="1"/>
+      <c r="BF13" s="4"/>
       <c r="BG13" s="1"/>
       <c r="BH13" s="1"/>
       <c r="BI13" s="1"/>
-    </row>
-    <row r="14" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ13" s="6">
+        <v>3</v>
+      </c>
+      <c r="BK13" s="1"/>
+      <c r="BL13" s="1"/>
+      <c r="BM13" s="1"/>
+      <c r="BN13" s="1"/>
+      <c r="BO13" s="1"/>
+    </row>
+    <row r="14" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="66" t="s">
         <v>61</v>
@@ -4631,7 +4718,9 @@
       <c r="AD14" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="AE14" s="1"/>
+      <c r="AE14" s="6">
+        <v>3</v>
+      </c>
       <c r="AF14" s="1"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="1"/>
@@ -4652,26 +4741,34 @@
       <c r="AS14" s="5"/>
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
-      <c r="AV14" s="1"/>
-      <c r="AW14" s="66" t="s">
+      <c r="AV14" s="66" t="s">
         <v>61</v>
       </c>
+      <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
-      <c r="AY14" s="1"/>
-      <c r="AZ14" s="5"/>
+      <c r="AY14" s="5"/>
+      <c r="AZ14" s="1"/>
       <c r="BA14" s="1"/>
       <c r="BB14" s="1"/>
-      <c r="BC14" s="1"/>
-      <c r="BD14" s="66" t="s">
+      <c r="BC14" s="66" t="s">
         <v>61</v>
       </c>
+      <c r="BD14" s="1"/>
       <c r="BE14" s="1"/>
-      <c r="BF14" s="1"/>
+      <c r="BF14" s="5"/>
       <c r="BG14" s="1"/>
       <c r="BH14" s="1"/>
       <c r="BI14" s="1"/>
-    </row>
-    <row r="15" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ14" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK14" s="1"/>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+      <c r="BO14" s="1"/>
+    </row>
+    <row r="15" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="8">
         <v>6</v>
@@ -4734,26 +4831,34 @@
       <c r="AS15" s="5"/>
       <c r="AT15" s="1"/>
       <c r="AU15" s="1"/>
-      <c r="AV15" s="1"/>
-      <c r="AW15" s="8">
+      <c r="AV15" s="8">
         <v>6</v>
       </c>
-      <c r="AX15" s="4"/>
+      <c r="AW15" s="4"/>
+      <c r="AX15" s="5"/>
       <c r="AY15" s="5"/>
-      <c r="AZ15" s="5"/>
+      <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
       <c r="BB15" s="1"/>
-      <c r="BC15" s="1"/>
-      <c r="BD15" s="8">
+      <c r="BC15" s="8">
         <v>6</v>
       </c>
-      <c r="BE15" s="4"/>
+      <c r="BD15" s="4"/>
+      <c r="BE15" s="5"/>
       <c r="BF15" s="5"/>
       <c r="BG15" s="1"/>
       <c r="BH15" s="1"/>
       <c r="BI15" s="1"/>
-    </row>
-    <row r="16" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ15" s="8">
+        <v>6</v>
+      </c>
+      <c r="BK15" s="4"/>
+      <c r="BL15" s="5"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+      <c r="BO15" s="1"/>
+    </row>
+    <row r="16" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="C16" s="6"/>
       <c r="D16" s="59" t="s">
@@ -4796,7 +4901,9 @@
       <c r="AE16" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="AF16" s="5"/>
+      <c r="AF16" s="21">
+        <v>2</v>
+      </c>
       <c r="AG16" s="5"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -4816,26 +4923,34 @@
       <c r="AS16" s="5"/>
       <c r="AT16" s="1"/>
       <c r="AU16" s="1"/>
-      <c r="AV16" s="1"/>
-      <c r="AW16" s="6"/>
-      <c r="AX16" s="59" t="s">
+      <c r="AV16" s="6"/>
+      <c r="AW16" s="59" t="s">
         <v>64</v>
       </c>
+      <c r="AX16" s="5"/>
       <c r="AY16" s="5"/>
-      <c r="AZ16" s="5"/>
+      <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
       <c r="BB16" s="1"/>
-      <c r="BC16" s="1"/>
-      <c r="BD16" s="6"/>
-      <c r="BE16" s="59" t="s">
+      <c r="BC16" s="6"/>
+      <c r="BD16" s="59" t="s">
         <v>64</v>
       </c>
+      <c r="BE16" s="5"/>
       <c r="BF16" s="5"/>
       <c r="BG16" s="1"/>
       <c r="BH16" s="1"/>
       <c r="BI16" s="1"/>
-    </row>
-    <row r="17" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ16" s="6"/>
+      <c r="BK16" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="BL16" s="5"/>
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+      <c r="BO16" s="1"/>
+    </row>
+    <row r="17" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="6">
         <v>2</v>
@@ -4898,26 +5013,34 @@
       <c r="AS17" s="1"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
-      <c r="AV17" s="1"/>
-      <c r="AW17" s="6">
+      <c r="AV17" s="6">
         <v>2</v>
       </c>
-      <c r="AX17" s="1"/>
-      <c r="AY17" s="4"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="4"/>
+      <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
       <c r="BA17" s="1"/>
       <c r="BB17" s="1"/>
-      <c r="BC17" s="1"/>
-      <c r="BD17" s="6">
+      <c r="BC17" s="6">
         <v>2</v>
       </c>
-      <c r="BE17" s="1"/>
-      <c r="BF17" s="4"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="4"/>
+      <c r="BF17" s="1"/>
       <c r="BG17" s="1"/>
       <c r="BH17" s="1"/>
       <c r="BI17" s="1"/>
-    </row>
-    <row r="18" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ17" s="6">
+        <v>2</v>
+      </c>
+      <c r="BK17" s="1"/>
+      <c r="BL17" s="4"/>
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+      <c r="BO17" s="1"/>
+    </row>
+    <row r="18" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="C18" s="66" t="s">
         <v>62</v>
@@ -4963,7 +5086,9 @@
       <c r="AD18" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="AE18" s="1"/>
+      <c r="AE18" s="6">
+        <v>2</v>
+      </c>
       <c r="AF18" s="5"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
@@ -4984,26 +5109,34 @@
       <c r="AS18" s="1"/>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
-      <c r="AV18" s="1"/>
-      <c r="AW18" s="66" t="s">
+      <c r="AV18" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="AX18" s="1"/>
-      <c r="AY18" s="5"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="5"/>
+      <c r="AY18" s="1"/>
       <c r="AZ18" s="1"/>
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
-      <c r="BC18" s="1"/>
-      <c r="BD18" s="66" t="s">
+      <c r="BC18" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="BE18" s="1"/>
-      <c r="BF18" s="5"/>
+      <c r="BD18" s="1"/>
+      <c r="BE18" s="5"/>
+      <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
       <c r="BI18" s="1"/>
-    </row>
-    <row r="19" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ18" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="BK18" s="1"/>
+      <c r="BL18" s="5"/>
+      <c r="BM18" s="1"/>
+      <c r="BN18" s="1"/>
+      <c r="BO18" s="1"/>
+    </row>
+    <row r="19" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="8">
         <v>7</v>
@@ -5066,34 +5199,42 @@
       <c r="AQ19" s="4"/>
       <c r="AR19" s="1"/>
       <c r="AS19" s="1"/>
-      <c r="AT19" s="1" t="s">
+      <c r="AT19" s="1"/>
+      <c r="AU19" s="1"/>
+      <c r="AV19" s="8">
+        <v>7</v>
+      </c>
+      <c r="AW19" s="4"/>
+      <c r="AX19" s="1"/>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AU19" s="1"/>
-      <c r="AV19" s="1"/>
-      <c r="AW19" s="8">
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="8">
         <v>7</v>
       </c>
-      <c r="AX19" s="4"/>
-      <c r="AY19" s="1"/>
-      <c r="AZ19" s="1"/>
-      <c r="BA19" s="1" t="s">
+      <c r="BD19" s="4"/>
+      <c r="BE19" s="1"/>
+      <c r="BF19" s="1"/>
+      <c r="BG19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BB19" s="1"/>
-      <c r="BC19" s="1"/>
-      <c r="BD19" s="8">
+      <c r="BH19" s="1"/>
+      <c r="BI19" s="1"/>
+      <c r="BJ19" s="8">
         <v>7</v>
       </c>
-      <c r="BE19" s="4"/>
-      <c r="BF19" s="1"/>
-      <c r="BG19" s="1"/>
-      <c r="BH19" s="1" t="s">
+      <c r="BK19" s="4"/>
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BI19" s="1"/>
-    </row>
-    <row r="20" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BO19" s="1"/>
+    </row>
+    <row r="20" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -5136,8 +5277,8 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
-      <c r="AF20" s="6" t="s">
-        <v>64</v>
+      <c r="AF20" s="6">
+        <v>3</v>
       </c>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
@@ -5145,7 +5286,7 @@
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
       <c r="AL20" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
@@ -5153,31 +5294,39 @@
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
       <c r="AR20" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AS20" s="1"/>
-      <c r="AT20" s="66"/>
-      <c r="AU20" s="5"/>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
-      <c r="AX20" s="1"/>
-      <c r="AY20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AZ20" s="1"/>
-      <c r="BA20" s="66"/>
-      <c r="BB20" s="5"/>
+      <c r="AX20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="66"/>
+      <c r="BA20" s="5"/>
+      <c r="BB20" s="1"/>
       <c r="BC20" s="1"/>
       <c r="BD20" s="1"/>
-      <c r="BE20" s="1"/>
-      <c r="BF20" s="6" t="s">
+      <c r="BE20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="BG20" s="1"/>
-      <c r="BH20" s="59"/>
+      <c r="BF20" s="1"/>
+      <c r="BG20" s="66"/>
+      <c r="BH20" s="5"/>
       <c r="BI20" s="1"/>
-    </row>
-    <row r="21" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ20" s="1"/>
+      <c r="BK20" s="1"/>
+      <c r="BL20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="BM20" s="1"/>
+      <c r="BN20" s="59"/>
+      <c r="BO20" s="1"/>
+    </row>
+    <row r="21" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -5217,13 +5366,15 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
-      <c r="AE21" s="6" t="s">
-        <v>59</v>
+      <c r="AE21" s="6">
+        <v>8</v>
       </c>
       <c r="AF21" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="AG21" s="1"/>
+      <c r="AG21" s="1">
+        <v>3</v>
+      </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
@@ -5238,44 +5389,54 @@
       <c r="AO21" s="1"/>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AR21" s="66" t="s">
         <v>81</v>
       </c>
       <c r="AS21" s="1"/>
-      <c r="AT21" s="59" t="s">
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX21" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="AU21" s="5"/>
-      <c r="AV21" s="1"/>
-      <c r="AW21" s="1"/>
-      <c r="AX21" s="6" t="s">
+      <c r="BA21" s="5"/>
+      <c r="BB21" s="1"/>
+      <c r="BC21" s="1"/>
+      <c r="BD21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AY21" s="66" t="s">
+      <c r="BE21" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="AZ21" s="1"/>
-      <c r="BA21" s="59" t="s">
+      <c r="BF21" s="1"/>
+      <c r="BG21" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="BB21" s="5"/>
-      <c r="BC21" s="1"/>
-      <c r="BD21" s="1"/>
-      <c r="BE21" s="6" t="s">
+      <c r="BH21" s="5"/>
+      <c r="BI21" s="1"/>
+      <c r="BJ21" s="1"/>
+      <c r="BK21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="BF21" s="66" t="s">
+      <c r="BL21" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="BG21" s="1"/>
-      <c r="BH21" s="59" t="s">
+      <c r="BM21" s="1"/>
+      <c r="BN21" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="BI21" s="1"/>
-    </row>
-    <row r="22" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BO21" s="1"/>
+    </row>
+    <row r="22" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -5318,7 +5479,9 @@
       <c r="AE22" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="AF22" s="8"/>
+      <c r="AF22" s="8">
+        <v>5</v>
+      </c>
       <c r="AG22" s="4"/>
       <c r="AH22" s="5"/>
       <c r="AI22" s="1"/>
@@ -5337,27 +5500,35 @@
       <c r="AR22" s="8"/>
       <c r="AS22" s="4"/>
       <c r="AT22" s="5"/>
-      <c r="AU22" s="4"/>
+      <c r="AU22" s="1"/>
       <c r="AV22" s="1"/>
-      <c r="AW22" s="1"/>
-      <c r="AX22" s="66" t="s">
+      <c r="AW22" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="AY22" s="8"/>
-      <c r="AZ22" s="4"/>
-      <c r="BA22" s="5"/>
-      <c r="BB22" s="4"/>
+      <c r="AX22" s="8"/>
+      <c r="AY22" s="4"/>
+      <c r="AZ22" s="5"/>
+      <c r="BA22" s="4"/>
+      <c r="BB22" s="1"/>
       <c r="BC22" s="1"/>
-      <c r="BD22" s="1"/>
-      <c r="BE22" s="66" t="s">
+      <c r="BD22" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="BF22" s="8"/>
-      <c r="BG22" s="4"/>
-      <c r="BH22" s="1"/>
+      <c r="BE22" s="8"/>
+      <c r="BF22" s="4"/>
+      <c r="BG22" s="5"/>
+      <c r="BH22" s="4"/>
       <c r="BI22" s="1"/>
-    </row>
-    <row r="23" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ22" s="1"/>
+      <c r="BK22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="BL22" s="8"/>
+      <c r="BM22" s="4"/>
+      <c r="BN22" s="1"/>
+      <c r="BO22" s="1"/>
+    </row>
+    <row r="23" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -5387,18 +5558,20 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
-      <c r="AE23" s="8" t="s">
-        <v>60</v>
+      <c r="AE23" s="8">
+        <v>5</v>
       </c>
       <c r="AF23" s="4"/>
       <c r="AG23" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="AH23" s="5"/>
+      <c r="AH23" s="5">
+        <v>3</v>
+      </c>
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AL23" s="4"/>
       <c r="AM23" s="59" t="s">
@@ -5408,36 +5581,46 @@
       <c r="AO23" s="1"/>
       <c r="AP23" s="1"/>
       <c r="AQ23" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AR23" s="4"/>
       <c r="AS23" s="59" t="s">
         <v>90</v>
       </c>
       <c r="AT23" s="5"/>
-      <c r="AU23" s="5"/>
+      <c r="AU23" s="1"/>
       <c r="AV23" s="1"/>
-      <c r="AW23" s="1"/>
-      <c r="AX23" s="8" t="s">
+      <c r="AW23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX23" s="4"/>
+      <c r="AY23" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ23" s="5"/>
+      <c r="BA23" s="5"/>
+      <c r="BB23" s="1"/>
+      <c r="BC23" s="1"/>
+      <c r="BD23" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AY23" s="4"/>
-      <c r="AZ23" s="59" t="s">
+      <c r="BE23" s="4"/>
+      <c r="BF23" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="BA23" s="5"/>
-      <c r="BB23" s="5"/>
-      <c r="BC23" s="1"/>
-      <c r="BD23" s="1"/>
-      <c r="BE23" s="8" t="s">
+      <c r="BG23" s="5"/>
+      <c r="BH23" s="5"/>
+      <c r="BI23" s="1"/>
+      <c r="BJ23" s="1"/>
+      <c r="BK23" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="BF23" s="4"/>
-      <c r="BG23" s="59"/>
-      <c r="BH23" s="1"/>
-      <c r="BI23" s="1"/>
-    </row>
-    <row r="24" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BL23" s="4"/>
+      <c r="BM23" s="59"/>
+      <c r="BN23" s="1"/>
+      <c r="BO23" s="1"/>
+    </row>
+    <row r="24" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -5468,8 +5651,8 @@
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
-      <c r="AF24" s="6" t="s">
-        <v>63</v>
+      <c r="AF24" s="6">
+        <v>4</v>
       </c>
       <c r="AG24" s="1"/>
       <c r="AH24" s="4"/>
@@ -5477,7 +5660,7 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM24" s="1"/>
       <c r="AN24" s="4"/>
@@ -5485,31 +5668,39 @@
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AS24" s="1"/>
       <c r="AT24" s="4"/>
       <c r="AU24" s="1"/>
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
-      <c r="AX24" s="1"/>
-      <c r="AY24" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ24" s="1"/>
-      <c r="BA24" s="4"/>
+      <c r="AX24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="4"/>
+      <c r="BA24" s="1"/>
       <c r="BB24" s="1"/>
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
-      <c r="BE24" s="1"/>
-      <c r="BF24" s="6" t="s">
+      <c r="BE24" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="BG24" s="1"/>
+      <c r="BF24" s="1"/>
+      <c r="BG24" s="4"/>
       <c r="BH24" s="1"/>
       <c r="BI24" s="1"/>
-    </row>
-    <row r="25" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ24" s="1"/>
+      <c r="BK24" s="1"/>
+      <c r="BL24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM24" s="1"/>
+      <c r="BN24" s="1"/>
+      <c r="BO24" s="1"/>
+    </row>
+    <row r="25" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -5539,18 +5730,20 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="6" t="s">
-        <v>61</v>
+      <c r="AE25" s="6">
+        <v>7</v>
       </c>
       <c r="AF25" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="AG25" s="1"/>
+      <c r="AG25" s="1">
+        <v>4</v>
+      </c>
       <c r="AH25" s="5"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AL25" s="66" t="s">
         <v>91</v>
@@ -5559,7 +5752,9 @@
       <c r="AN25" s="5"/>
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
-      <c r="AQ25" s="6"/>
+      <c r="AQ25" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="AR25" s="66" t="s">
         <v>91</v>
       </c>
@@ -5567,29 +5762,37 @@
       <c r="AT25" s="5"/>
       <c r="AU25" s="1"/>
       <c r="AV25" s="1"/>
-      <c r="AW25" s="1"/>
-      <c r="AX25" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY25" s="66" t="s">
+      <c r="AW25" s="6"/>
+      <c r="AX25" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="AZ25" s="1"/>
-      <c r="BA25" s="5"/>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="5"/>
+      <c r="BA25" s="1"/>
       <c r="BB25" s="1"/>
       <c r="BC25" s="1"/>
-      <c r="BD25" s="1"/>
-      <c r="BE25" s="6" t="s">
+      <c r="BD25" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="BF25" s="66" t="s">
+      <c r="BE25" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="BG25" s="1"/>
+      <c r="BF25" s="1"/>
+      <c r="BG25" s="5"/>
       <c r="BH25" s="1"/>
       <c r="BI25" s="1"/>
-    </row>
-    <row r="26" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ25" s="1"/>
+      <c r="BK25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="BL25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM25" s="1"/>
+      <c r="BN25" s="1"/>
+      <c r="BO25" s="1"/>
+    </row>
+    <row r="26" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -5622,7 +5825,9 @@
       <c r="AE26" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="AF26" s="8"/>
+      <c r="AF26" s="8">
+        <v>6</v>
+      </c>
       <c r="AG26" s="4"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
@@ -5635,33 +5840,41 @@
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
       <c r="AP26" s="1"/>
-      <c r="AQ26" s="59"/>
-      <c r="AR26" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="AQ26" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR26" s="8"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
-      <c r="AW26" s="1"/>
-      <c r="AX26" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="AY26" s="8"/>
-      <c r="AZ26" s="4"/>
+      <c r="AW26" s="59"/>
+      <c r="AX26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AY26" s="4"/>
+      <c r="AZ26" s="1"/>
       <c r="BA26" s="1"/>
       <c r="BB26" s="1"/>
       <c r="BC26" s="1"/>
-      <c r="BD26" s="1"/>
-      <c r="BE26" s="66" t="s">
+      <c r="BD26" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="BF26" s="8"/>
-      <c r="BG26" s="4"/>
+      <c r="BE26" s="8"/>
+      <c r="BF26" s="4"/>
+      <c r="BG26" s="1"/>
       <c r="BH26" s="1"/>
       <c r="BI26" s="1"/>
-    </row>
-    <row r="27" spans="2:61" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ26" s="1"/>
+      <c r="BK26" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="BL26" s="8"/>
+      <c r="BM26" s="4"/>
+      <c r="BN26" s="1"/>
+      <c r="BO26" s="1"/>
+    </row>
+    <row r="27" spans="2:67" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -5691,8 +5904,8 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
-      <c r="AE27" s="8" t="s">
-        <v>62</v>
+      <c r="AE27" s="8">
+        <v>6</v>
       </c>
       <c r="AF27" s="4"/>
       <c r="AG27" s="1"/>
@@ -5707,31 +5920,39 @@
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
       <c r="AP27" s="1"/>
-      <c r="AQ27" s="6"/>
-      <c r="AR27" s="9"/>
+      <c r="AQ27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR27" s="4"/>
       <c r="AS27" s="1"/>
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
       <c r="AV27" s="1"/>
-      <c r="AW27" s="1"/>
-      <c r="AX27" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AY27" s="4"/>
+      <c r="AW27" s="6"/>
+      <c r="AX27" s="9"/>
+      <c r="AY27" s="1"/>
       <c r="AZ27" s="1"/>
       <c r="BA27" s="1"/>
       <c r="BB27" s="1"/>
       <c r="BC27" s="1"/>
-      <c r="BD27" s="1"/>
-      <c r="BE27" s="8" t="s">
+      <c r="BD27" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BF27" s="4"/>
+      <c r="BE27" s="4"/>
+      <c r="BF27" s="1"/>
       <c r="BG27" s="1"/>
       <c r="BH27" s="1"/>
       <c r="BI27" s="1"/>
-    </row>
-    <row r="28" spans="2:61" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="BJ27" s="1"/>
+      <c r="BK27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL27" s="4"/>
+      <c r="BM27" s="1"/>
+      <c r="BN27" s="1"/>
+      <c r="BO27" s="1"/>
+    </row>
+    <row r="28" spans="2:67" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -5792,6 +6013,12 @@
       <c r="BG28" s="1"/>
       <c r="BH28" s="1"/>
       <c r="BI28" s="1"/>
+      <c r="BJ28" s="1"/>
+      <c r="BK28" s="1"/>
+      <c r="BL28" s="1"/>
+      <c r="BM28" s="1"/>
+      <c r="BN28" s="1"/>
+      <c r="BO28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6875,7 +7102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D84D55B-86DB-41A7-86B6-8D3E6C4FEE99}">
   <dimension ref="C4:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14:H28"/>
     </sheetView>
   </sheetViews>
@@ -7436,15 +7663,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A138887D-E83F-4832-AC66-DEE1E0C0D3AC}">
-  <dimension ref="A4:AC33"/>
+  <dimension ref="A4:AH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="AH23" sqref="AH23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -7475,7 +7702,7 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -7526,7 +7753,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -7569,7 +7796,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -7604,7 +7831,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="7"/>
@@ -7637,7 +7864,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
@@ -7672,7 +7899,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -7711,7 +7938,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
-    <row r="11" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -7746,7 +7973,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
-    <row r="12" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>111</v>
@@ -7778,8 +8005,13 @@
       <c r="AA12" s="90"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
-    </row>
-    <row r="13" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="7"/>
       <c r="C13" s="1"/>
@@ -7813,8 +8045,13 @@
       <c r="AA13" s="90"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
         <v>111</v>
@@ -7839,15 +8076,22 @@
       <c r="T14" s="4"/>
       <c r="U14" s="90"/>
       <c r="V14" s="90"/>
-      <c r="W14" s="90"/>
-      <c r="X14" s="90"/>
-      <c r="Y14" s="90"/>
-      <c r="Z14" s="90"/>
-      <c r="AA14" s="90"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -7872,15 +8116,22 @@
       <c r="T15" s="5"/>
       <c r="U15" s="90"/>
       <c r="V15" s="90"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="90"/>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="90"/>
-      <c r="AA15" s="90"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
-    </row>
-    <row r="16" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -7905,15 +8156,24 @@
       <c r="T16" s="5"/>
       <c r="U16" s="90"/>
       <c r="V16" s="90"/>
-      <c r="W16" s="90"/>
-      <c r="X16" s="90"/>
-      <c r="Y16" s="90"/>
-      <c r="Z16" s="90"/>
-      <c r="AA16" s="90"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-    </row>
-    <row r="17" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -7938,15 +8198,20 @@
       <c r="T17" s="5"/>
       <c r="U17" s="90"/>
       <c r="V17" s="90"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="90"/>
-      <c r="Y17" s="90"/>
-      <c r="Z17" s="90"/>
-      <c r="AA17" s="90"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="5"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -7969,15 +8234,24 @@
       <c r="T18" s="1"/>
       <c r="U18" s="90"/>
       <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="5"/>
       <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -8002,15 +8276,22 @@
       <c r="T19" s="1"/>
       <c r="U19" s="90"/>
       <c r="V19" s="90"/>
-      <c r="W19" s="90"/>
-      <c r="X19" s="90"/>
-      <c r="Y19" s="90"/>
-      <c r="Z19" s="90"/>
-      <c r="AA19" s="90"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="4"/>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="20" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -8037,15 +8318,24 @@
       <c r="T20" s="1"/>
       <c r="U20" s="90"/>
       <c r="V20" s="90"/>
-      <c r="W20" s="91"/>
-      <c r="X20" s="90"/>
-      <c r="Y20" s="90"/>
-      <c r="Z20" s="90"/>
-      <c r="AA20" s="90"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="5"/>
       <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+    </row>
+    <row r="21" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -8070,15 +8360,20 @@
       <c r="T21" s="90"/>
       <c r="U21" s="90"/>
       <c r="V21" s="91"/>
-      <c r="W21" s="91"/>
-      <c r="X21" s="90"/>
-      <c r="Y21" s="90"/>
-      <c r="Z21" s="90"/>
-      <c r="AA21" s="90"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-    <row r="22" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="6" t="s">
@@ -8107,15 +8402,24 @@
       <c r="T22" s="93"/>
       <c r="U22" s="90"/>
       <c r="V22" s="91"/>
-      <c r="W22" s="90"/>
-      <c r="X22" s="90"/>
-      <c r="Y22" s="90"/>
-      <c r="Z22" s="90"/>
-      <c r="AA22" s="90"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-    </row>
-    <row r="23" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="7"/>
@@ -8137,18 +8441,22 @@
       <c r="S23" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="T23" s="1"/>
       <c r="U23" s="90"/>
       <c r="V23" s="91"/>
-      <c r="W23" s="90"/>
-      <c r="X23" s="90"/>
-      <c r="Y23" s="90"/>
-      <c r="Z23" s="90"/>
-      <c r="AA23" s="90"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-    </row>
-    <row r="24" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+    </row>
+    <row r="24" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="8" t="s">
@@ -8174,18 +8482,24 @@
       <c r="S24" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="T24" s="4"/>
       <c r="U24" s="90"/>
       <c r="V24" s="91"/>
-      <c r="W24" s="91"/>
-      <c r="X24" s="90"/>
-      <c r="Y24" s="90"/>
-      <c r="Z24" s="90"/>
-      <c r="AA24" s="90"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-    </row>
-    <row r="25" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -8210,15 +8524,20 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="91"/>
-      <c r="W25" s="90"/>
-      <c r="X25" s="90"/>
-      <c r="Y25" s="90"/>
-      <c r="Z25" s="90"/>
-      <c r="AA25" s="90"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-    </row>
-    <row r="26" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+    </row>
+    <row r="26" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="6" t="s">
@@ -8240,9 +8559,9 @@
       <c r="O26" s="90"/>
       <c r="P26" s="90"/>
       <c r="Q26" s="91"/>
-      <c r="R26" s="91"/>
+      <c r="R26" s="6"/>
       <c r="S26" s="90"/>
-      <c r="T26" s="90"/>
+      <c r="T26" s="1"/>
       <c r="U26" s="90"/>
       <c r="V26" s="91"/>
       <c r="W26" s="90"/>
@@ -8252,8 +8571,13 @@
       <c r="AA26" s="90"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
-    </row>
-    <row r="27" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+    </row>
+    <row r="27" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="7"/>
@@ -8270,7 +8594,7 @@
       <c r="N27" s="90"/>
       <c r="O27" s="90"/>
       <c r="P27" s="90"/>
-      <c r="Q27" s="91"/>
+      <c r="Q27" s="90"/>
       <c r="R27" s="90"/>
       <c r="S27" s="90"/>
       <c r="T27" s="90"/>
@@ -8283,8 +8607,13 @@
       <c r="AA27" s="90"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-    </row>
-    <row r="28" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
@@ -8305,7 +8634,7 @@
       <c r="N28" s="90"/>
       <c r="O28" s="90"/>
       <c r="P28" s="90"/>
-      <c r="Q28" s="91"/>
+      <c r="Q28" s="90"/>
       <c r="R28" s="90"/>
       <c r="S28" s="90"/>
       <c r="T28" s="90"/>
@@ -8319,7 +8648,7 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
-    <row r="29" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -8336,9 +8665,11 @@
       <c r="N29" s="90"/>
       <c r="O29" s="90"/>
       <c r="P29" s="90"/>
-      <c r="Q29" s="90"/>
-      <c r="R29" s="90"/>
-      <c r="S29" s="90"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="S29" s="5"/>
       <c r="T29" s="90"/>
       <c r="U29" s="90"/>
       <c r="V29" s="91"/>
@@ -8350,7 +8681,7 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
-    <row r="30" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -8369,10 +8700,12 @@
       <c r="N30" s="90"/>
       <c r="O30" s="90"/>
       <c r="P30" s="90"/>
-      <c r="Q30" s="90"/>
-      <c r="R30" s="90"/>
-      <c r="S30" s="90"/>
-      <c r="T30" s="90"/>
+      <c r="Q30" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" s="1"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="5"/>
       <c r="U30" s="90"/>
       <c r="V30" s="91"/>
       <c r="W30" s="90"/>
@@ -8383,7 +8716,7 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
-    <row r="31" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -8396,14 +8729,14 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="M31" s="90"/>
       <c r="N31" s="90"/>
       <c r="O31" s="90"/>
-      <c r="P31" s="90"/>
-      <c r="Q31" s="90"/>
-      <c r="R31" s="90"/>
-      <c r="S31" s="90"/>
-      <c r="T31" s="90"/>
+      <c r="P31" s="91"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="5"/>
       <c r="U31" s="90"/>
       <c r="V31" s="90"/>
       <c r="W31" s="90"/>
@@ -8414,7 +8747,7 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -8427,14 +8760,16 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="M32" s="90"/>
       <c r="N32" s="90"/>
       <c r="O32" s="90"/>
-      <c r="P32" s="90"/>
-      <c r="Q32" s="90"/>
-      <c r="R32" s="90"/>
-      <c r="S32" s="90"/>
-      <c r="T32" s="90"/>
+      <c r="P32" s="91"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="T32" s="5"/>
       <c r="U32" s="90"/>
       <c r="V32" s="90"/>
       <c r="W32" s="90"/>
@@ -8445,7 +8780,7 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -8458,14 +8793,16 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="M33" s="90"/>
       <c r="N33" s="90"/>
       <c r="O33" s="90"/>
-      <c r="P33" s="90"/>
-      <c r="Q33" s="90"/>
-      <c r="R33" s="90"/>
-      <c r="S33" s="90"/>
-      <c r="T33" s="90"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="4"/>
       <c r="U33" s="90"/>
       <c r="V33" s="90"/>
       <c r="W33" s="90"/>
@@ -8475,6 +8812,189 @@
       <c r="AA33" s="90"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
+    </row>
+    <row r="34" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="90"/>
+      <c r="P34" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q34" s="92"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="90"/>
+      <c r="V34" s="90"/>
+      <c r="W34" s="90"/>
+    </row>
+    <row r="35" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="90"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="90"/>
+      <c r="V35" s="90"/>
+      <c r="W35" s="90"/>
+    </row>
+    <row r="36" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M36" s="90"/>
+      <c r="N36" s="90"/>
+      <c r="O36" s="90"/>
+      <c r="P36" s="90"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="90"/>
+      <c r="V36" s="90"/>
+      <c r="W36" s="90"/>
+    </row>
+    <row r="37" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M37" s="90"/>
+      <c r="N37" s="90"/>
+      <c r="O37" s="90"/>
+      <c r="P37" s="91"/>
+      <c r="Q37" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="R37" s="1"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="90"/>
+      <c r="V37" s="90"/>
+      <c r="W37" s="90"/>
+    </row>
+    <row r="38" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M38" s="90"/>
+      <c r="N38" s="90"/>
+      <c r="O38" s="90"/>
+      <c r="P38" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q38" s="92"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="90"/>
+      <c r="V38" s="90"/>
+      <c r="W38" s="90"/>
+    </row>
+    <row r="39" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M39" s="90"/>
+      <c r="N39" s="90"/>
+      <c r="O39" s="90"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="90"/>
+      <c r="T39" s="90"/>
+      <c r="U39" s="90"/>
+      <c r="V39" s="90"/>
+      <c r="W39" s="90"/>
+    </row>
+    <row r="40" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M40" s="90"/>
+      <c r="N40" s="90"/>
+      <c r="O40" s="90"/>
+      <c r="P40" s="90"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T40" s="93"/>
+      <c r="U40" s="90"/>
+      <c r="V40" s="90"/>
+      <c r="W40" s="90"/>
+    </row>
+    <row r="41" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M41" s="90"/>
+      <c r="N41" s="90"/>
+      <c r="O41" s="90"/>
+      <c r="P41" s="90"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="T41" s="1"/>
+      <c r="U41" s="90"/>
+      <c r="V41" s="90"/>
+      <c r="W41" s="90"/>
+    </row>
+    <row r="42" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M42" s="90"/>
+      <c r="N42" s="90"/>
+      <c r="O42" s="90"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="91"/>
+      <c r="R42" s="90"/>
+      <c r="S42" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="T42" s="4"/>
+      <c r="U42" s="90"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
+    </row>
+    <row r="43" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="M43" s="90"/>
+      <c r="N43" s="90"/>
+      <c r="O43" s="90"/>
+      <c r="P43" s="90"/>
+      <c r="Q43" s="90"/>
+      <c r="R43" s="90"/>
+      <c r="S43" s="90"/>
+      <c r="T43" s="90"/>
+      <c r="U43" s="90"/>
+      <c r="V43" s="90"/>
+      <c r="W43" s="90"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="M44" s="90"/>
+      <c r="N44" s="90"/>
+      <c r="O44" s="90"/>
+      <c r="P44" s="90"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="90"/>
+      <c r="S44" s="90"/>
+      <c r="T44" s="90"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="90"/>
+      <c r="W44" s="90"/>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="M45" s="90"/>
+      <c r="N45" s="90"/>
+      <c r="O45" s="90"/>
+      <c r="P45" s="90"/>
+      <c r="Q45" s="90"/>
+      <c r="R45" s="90"/>
+      <c r="S45" s="90"/>
+      <c r="T45" s="90"/>
+      <c r="U45" s="90"/>
+      <c r="V45" s="90"/>
+      <c r="W45" s="90"/>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="M46" s="90"/>
+      <c r="N46" s="90"/>
+      <c r="O46" s="90"/>
+      <c r="P46" s="90"/>
+      <c r="Q46" s="90"/>
+      <c r="R46" s="90"/>
+      <c r="S46" s="90"/>
+      <c r="T46" s="90"/>
+      <c r="U46" s="90"/>
+      <c r="V46" s="90"/>
+      <c r="W46" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10188,6 +10708,577 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DB49D5-2BEF-4B19-896A-64C90AC94C6F}">
+  <dimension ref="B2:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+      <c r="C5" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="C17" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="8"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10739,7 +11830,7 @@
   <dimension ref="A5:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E14"/>
+      <selection activeCell="K5" sqref="A5:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Quick edits to multibrackets before sending
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8B1185-7C86-45A4-AC67-6F462D7F92A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C83B625-F1BE-417E-8334-5C55C9E57AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="12" activeTab="22" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="13" activeTab="23" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="Sheet20" sheetId="22" r:id="rId21"/>
     <sheet name="Sheet21" sheetId="23" r:id="rId22"/>
     <sheet name="Sheet22" sheetId="24" r:id="rId23"/>
+    <sheet name="Sheet23" sheetId="25" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="139">
   <si>
     <t>Georgia</t>
   </si>
@@ -452,6 +453,30 @@
   <si>
     <t>C2</t>
   </si>
+  <si>
+    <t>X-j</t>
+  </si>
+  <si>
+    <t>X-i</t>
+  </si>
+  <si>
+    <t>1v2</t>
+  </si>
+  <si>
+    <t>1v3</t>
+  </si>
+  <si>
+    <t>4v2</t>
+  </si>
+  <si>
+    <t>4v3</t>
+  </si>
+  <si>
+    <t>pkj*W(x-j)</t>
+  </si>
+  <si>
+    <t>pki*W(x-i)</t>
+  </si>
 </sst>
 </file>
 
@@ -487,7 +512,7 @@
       <family val="4"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +546,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,7 +948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1043,10 +1074,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1055,13 +1092,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1070,16 +1104,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3286,7 +3311,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="85" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3295,7 +3320,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="84"/>
+      <c r="D11" s="86"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3341,7 +3366,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="85" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3350,7 +3375,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="84"/>
+      <c r="D18" s="86"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -7123,16 +7148,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="90"/>
       <c r="F5" s="67"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="88" t="s">
+      <c r="H5" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="89"/>
+      <c r="I5" s="90"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -7771,12 +7796,12 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90">
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1">
         <v>5</v>
       </c>
-      <c r="Q6" s="90">
+      <c r="Q6" s="1">
         <v>4</v>
       </c>
       <c r="R6" s="1">
@@ -7786,13 +7811,13 @@
         <v>1</v>
       </c>
       <c r="T6" s="1"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="91"/>
-      <c r="Y6" s="90"/>
-      <c r="Z6" s="90"/>
-      <c r="AA6" s="90"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
     </row>
@@ -7814,20 +7839,20 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="91"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="90"/>
-      <c r="AA7" s="90"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
     </row>
@@ -7847,20 +7872,20 @@
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="91"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
-      <c r="S8" s="90"/>
+      <c r="S8" s="1"/>
       <c r="T8" s="1"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
-      <c r="W8" s="91"/>
-      <c r="X8" s="90"/>
-      <c r="Y8" s="90"/>
-      <c r="Z8" s="90"/>
-      <c r="AA8" s="90"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
     </row>
@@ -7880,22 +7905,22 @@
       <c r="K9" s="1"/>
       <c r="L9" s="5"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="66" t="s">
         <v>65</v>
       </c>
       <c r="S9" s="5"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="91"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="90"/>
-      <c r="Y9" s="90"/>
-      <c r="Z9" s="90"/>
-      <c r="AA9" s="90"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
     </row>
@@ -7919,22 +7944,22 @@
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="90"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
       <c r="Q10" s="66" t="s">
         <v>63</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="4"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="91"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="91"/>
-      <c r="Y10" s="90"/>
-      <c r="Z10" s="90"/>
-      <c r="AA10" s="90"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
     </row>
@@ -7956,20 +7981,20 @@
       <c r="K11" s="1"/>
       <c r="L11" s="5"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="90"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="4"/>
       <c r="S11" s="1"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="90"/>
-      <c r="X11" s="91"/>
-      <c r="Y11" s="90"/>
-      <c r="Z11" s="90"/>
-      <c r="AA11" s="90"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
     </row>
@@ -7989,20 +8014,20 @@
       <c r="K12" s="4"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="91"/>
-      <c r="X12" s="90"/>
-      <c r="Y12" s="90"/>
-      <c r="Z12" s="90"/>
-      <c r="AA12" s="90"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
@@ -8027,22 +8052,22 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="91"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="1"/>
       <c r="S13" s="59" t="s">
         <v>66</v>
       </c>
       <c r="T13" s="5"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="91"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="90"/>
-      <c r="AA13" s="90"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -8067,15 +8092,15 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="91"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -8105,17 +8130,17 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="90"/>
-      <c r="O15" s="90"/>
-      <c r="P15" s="91"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="6"/>
       <c r="Q15" s="66" t="s">
         <v>64</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="5"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1" t="s">
@@ -8145,17 +8170,17 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
       <c r="P16" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="Q16" s="92"/>
+      <c r="Q16" s="81"/>
       <c r="R16" s="4"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="90"/>
-      <c r="V16" s="90"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1" t="s">
         <v>64</v>
@@ -8187,8 +8212,8 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="90"/>
-      <c r="O17" s="90"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="59" t="s">
@@ -8196,8 +8221,8 @@
       </c>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="90"/>
-      <c r="V17" s="90"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="1"/>
@@ -8225,15 +8250,15 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="1"/>
       <c r="S18" s="4"/>
       <c r="T18" s="1"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="3" t="s">
         <v>60</v>
@@ -8265,17 +8290,17 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="90"/>
-      <c r="O19" s="90"/>
-      <c r="P19" s="91"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="66" t="s">
         <v>129</v>
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="5"/>
       <c r="T19" s="1"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="90"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1" t="s">
@@ -8307,17 +8332,17 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="90"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
       <c r="P20" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="Q20" s="92"/>
+      <c r="Q20" s="81"/>
       <c r="R20" s="4"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1" t="s">
         <v>129</v>
@@ -8351,15 +8376,15 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="90"/>
-      <c r="O21" s="90"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
-      <c r="S21" s="90"/>
-      <c r="T21" s="90"/>
-      <c r="U21" s="90"/>
-      <c r="V21" s="91"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="6"/>
       <c r="W21" s="1"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="1"/>
@@ -8391,17 +8416,17 @@
       <c r="K22" s="5"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="90"/>
-      <c r="O22" s="90"/>
-      <c r="P22" s="90"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T22" s="93"/>
-      <c r="U22" s="90"/>
-      <c r="V22" s="91"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="6"/>
       <c r="W22" s="1"/>
       <c r="X22" s="3" t="s">
         <v>59</v>
@@ -8433,16 +8458,16 @@
       <c r="K23" s="5"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="90"/>
-      <c r="O23" s="90"/>
-      <c r="P23" s="90"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="U23" s="90"/>
-      <c r="V23" s="91"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="6"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -8474,16 +8499,16 @@
       <c r="K24" s="5"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="90"/>
-      <c r="O24" s="90"/>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="91"/>
-      <c r="R24" s="90"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="1"/>
       <c r="S24" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="U24" s="90"/>
-      <c r="V24" s="91"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="6"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
@@ -8515,15 +8540,15 @@
       <c r="K25" s="4"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="90"/>
-      <c r="O25" s="90"/>
-      <c r="P25" s="90"/>
-      <c r="Q25" s="90"/>
-      <c r="R25" s="91"/>
-      <c r="S25" s="90"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="V25" s="91"/>
+      <c r="V25" s="6"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -8555,20 +8580,20 @@
       <c r="K26" s="5"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="90"/>
-      <c r="O26" s="90"/>
-      <c r="P26" s="90"/>
-      <c r="Q26" s="91"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="90"/>
+      <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="90"/>
-      <c r="V26" s="91"/>
-      <c r="W26" s="90"/>
-      <c r="X26" s="90"/>
-      <c r="Y26" s="90"/>
-      <c r="Z26" s="90"/>
-      <c r="AA26" s="90"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
@@ -8591,20 +8616,20 @@
       <c r="K27" s="5"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="N27" s="90"/>
-      <c r="O27" s="90"/>
-      <c r="P27" s="90"/>
-      <c r="Q27" s="90"/>
-      <c r="R27" s="90"/>
-      <c r="S27" s="90"/>
-      <c r="T27" s="90"/>
-      <c r="U27" s="90"/>
-      <c r="V27" s="90"/>
-      <c r="W27" s="90"/>
-      <c r="X27" s="90"/>
-      <c r="Y27" s="90"/>
-      <c r="Z27" s="90"/>
-      <c r="AA27" s="90"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
@@ -8631,20 +8656,20 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="90"/>
-      <c r="Q28" s="90"/>
-      <c r="R28" s="90"/>
-      <c r="S28" s="90"/>
-      <c r="T28" s="90"/>
-      <c r="U28" s="90"/>
-      <c r="V28" s="91"/>
-      <c r="W28" s="90"/>
-      <c r="X28" s="90"/>
-      <c r="Y28" s="90"/>
-      <c r="Z28" s="90"/>
-      <c r="AA28" s="90"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
     </row>
@@ -8662,22 +8687,22 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="90"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="66" t="s">
         <v>65</v>
       </c>
       <c r="S29" s="5"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="90"/>
-      <c r="V29" s="91"/>
-      <c r="W29" s="90"/>
-      <c r="X29" s="90"/>
-      <c r="Y29" s="90"/>
-      <c r="Z29" s="90"/>
-      <c r="AA29" s="90"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
     </row>
@@ -8697,22 +8722,22 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="90"/>
-      <c r="O30" s="90"/>
-      <c r="P30" s="90"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="66" t="s">
         <v>63</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="4"/>
       <c r="T30" s="5"/>
-      <c r="U30" s="90"/>
-      <c r="V30" s="91"/>
-      <c r="W30" s="90"/>
-      <c r="X30" s="90"/>
-      <c r="Y30" s="90"/>
-      <c r="Z30" s="90"/>
-      <c r="AA30" s="90"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
     </row>
@@ -8729,21 +8754,21 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="90"/>
-      <c r="O31" s="90"/>
-      <c r="P31" s="91"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="6"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="4"/>
       <c r="S31" s="1"/>
       <c r="T31" s="5"/>
-      <c r="U31" s="90"/>
-      <c r="V31" s="90"/>
-      <c r="W31" s="90"/>
-      <c r="X31" s="90"/>
-      <c r="Y31" s="90"/>
-      <c r="Z31" s="90"/>
-      <c r="AA31" s="90"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
     </row>
@@ -8760,23 +8785,23 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="90"/>
-      <c r="N32" s="90"/>
-      <c r="O32" s="90"/>
-      <c r="P32" s="91"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="1"/>
       <c r="S32" s="59" t="s">
         <v>66</v>
       </c>
       <c r="T32" s="5"/>
-      <c r="U32" s="90"/>
-      <c r="V32" s="90"/>
-      <c r="W32" s="90"/>
-      <c r="X32" s="90"/>
-      <c r="Y32" s="90"/>
-      <c r="Z32" s="90"/>
-      <c r="AA32" s="90"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
     </row>
@@ -8793,45 +8818,45 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="90"/>
-      <c r="O33" s="90"/>
-      <c r="P33" s="91"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="6"/>
       <c r="Q33" s="66" t="s">
         <v>64</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="4"/>
-      <c r="U33" s="90"/>
-      <c r="V33" s="90"/>
-      <c r="W33" s="90"/>
-      <c r="X33" s="90"/>
-      <c r="Y33" s="90"/>
-      <c r="Z33" s="90"/>
-      <c r="AA33" s="90"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
     </row>
     <row r="34" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M34" s="90"/>
-      <c r="N34" s="90"/>
-      <c r="O34" s="90"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
       <c r="P34" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="Q34" s="92"/>
+      <c r="Q34" s="81"/>
       <c r="R34" s="4"/>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
-      <c r="U34" s="90"/>
-      <c r="V34" s="90"/>
-      <c r="W34" s="90"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
     </row>
     <row r="35" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M35" s="90"/>
-      <c r="N35" s="90"/>
-      <c r="O35" s="90"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="59" t="s">
@@ -8839,162 +8864,162 @@
       </c>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
-      <c r="U35" s="90"/>
-      <c r="V35" s="90"/>
-      <c r="W35" s="90"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
     </row>
     <row r="36" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M36" s="90"/>
-      <c r="N36" s="90"/>
-      <c r="O36" s="90"/>
-      <c r="P36" s="90"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="1"/>
       <c r="S36" s="4"/>
       <c r="T36" s="1"/>
-      <c r="U36" s="90"/>
-      <c r="V36" s="90"/>
-      <c r="W36" s="90"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
     </row>
     <row r="37" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M37" s="90"/>
-      <c r="N37" s="90"/>
-      <c r="O37" s="90"/>
-      <c r="P37" s="91"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="6"/>
       <c r="Q37" s="66" t="s">
         <v>129</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="5"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="90"/>
-      <c r="V37" s="90"/>
-      <c r="W37" s="90"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
     </row>
     <row r="38" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M38" s="90"/>
-      <c r="N38" s="90"/>
-      <c r="O38" s="90"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
       <c r="P38" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="Q38" s="92"/>
+      <c r="Q38" s="81"/>
       <c r="R38" s="4"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-      <c r="U38" s="90"/>
-      <c r="V38" s="90"/>
-      <c r="W38" s="90"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
     </row>
     <row r="39" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M39" s="90"/>
-      <c r="N39" s="90"/>
-      <c r="O39" s="90"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
       <c r="P39" s="8"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="90"/>
-      <c r="T39" s="90"/>
-      <c r="U39" s="90"/>
-      <c r="V39" s="90"/>
-      <c r="W39" s="90"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
     </row>
     <row r="40" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M40" s="90"/>
-      <c r="N40" s="90"/>
-      <c r="O40" s="90"/>
-      <c r="P40" s="90"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T40" s="93"/>
-      <c r="U40" s="90"/>
-      <c r="V40" s="90"/>
-      <c r="W40" s="90"/>
+      <c r="T40" s="59"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M41" s="90"/>
-      <c r="N41" s="90"/>
-      <c r="O41" s="90"/>
-      <c r="P41" s="90"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="66" t="s">
         <v>81</v>
       </c>
       <c r="T41" s="1"/>
-      <c r="U41" s="90"/>
-      <c r="V41" s="90"/>
-      <c r="W41" s="90"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:29" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M42" s="90"/>
-      <c r="N42" s="90"/>
-      <c r="O42" s="90"/>
-      <c r="P42" s="90"/>
-      <c r="Q42" s="91"/>
-      <c r="R42" s="90"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="1"/>
       <c r="S42" s="8" t="s">
         <v>130</v>
       </c>
       <c r="T42" s="4"/>
-      <c r="U42" s="90"/>
-      <c r="V42" s="90"/>
-      <c r="W42" s="90"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="M43" s="90"/>
-      <c r="N43" s="90"/>
-      <c r="O43" s="90"/>
-      <c r="P43" s="90"/>
-      <c r="Q43" s="90"/>
-      <c r="R43" s="90"/>
-      <c r="S43" s="90"/>
-      <c r="T43" s="90"/>
-      <c r="U43" s="90"/>
-      <c r="V43" s="90"/>
-      <c r="W43" s="90"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="M44" s="90"/>
-      <c r="N44" s="90"/>
-      <c r="O44" s="90"/>
-      <c r="P44" s="90"/>
-      <c r="Q44" s="90"/>
-      <c r="R44" s="90"/>
-      <c r="S44" s="90"/>
-      <c r="T44" s="90"/>
-      <c r="U44" s="90"/>
-      <c r="V44" s="90"/>
-      <c r="W44" s="90"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="M45" s="90"/>
-      <c r="N45" s="90"/>
-      <c r="O45" s="90"/>
-      <c r="P45" s="90"/>
-      <c r="Q45" s="90"/>
-      <c r="R45" s="90"/>
-      <c r="S45" s="90"/>
-      <c r="T45" s="90"/>
-      <c r="U45" s="90"/>
-      <c r="V45" s="90"/>
-      <c r="W45" s="90"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="M46" s="90"/>
-      <c r="N46" s="90"/>
-      <c r="O46" s="90"/>
-      <c r="P46" s="90"/>
-      <c r="Q46" s="90"/>
-      <c r="R46" s="90"/>
-      <c r="S46" s="90"/>
-      <c r="T46" s="90"/>
-      <c r="U46" s="90"/>
-      <c r="V46" s="90"/>
-      <c r="W46" s="90"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10716,7 +10741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DB49D5-2BEF-4B19-896A-64C90AC94C6F}">
   <dimension ref="B2:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
@@ -11277,6 +11302,633 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887B89AA-C696-4373-8C0A-DD193E62BDA9}">
+  <dimension ref="C5:AC25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="91">
+        <f>1-E9</f>
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="91">
+        <f>1-E10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="91">
+        <f>1-E11</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="91" t="b">
+        <f>AND(E8&lt;=F8,F8&lt;=G8,G8&lt;=H8)</f>
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="T8" s="91">
+        <f>1-S9</f>
+        <v>0.8</v>
+      </c>
+      <c r="U8" s="91">
+        <f>1-S10</f>
+        <v>0.8</v>
+      </c>
+      <c r="V8" s="91">
+        <f>1-S11</f>
+        <v>0.9</v>
+      </c>
+      <c r="X8" s="91" t="b">
+        <f>AND(S8&lt;=T8,T8&lt;=U8,U8&lt;=V8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="91">
+        <f>1-F10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="91">
+        <f>1-F11</f>
+        <v>0.8</v>
+      </c>
+      <c r="J9" s="91" t="b">
+        <f>AND(E9&lt;=F9,F9&lt;=G9,G9&lt;=H9)</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>0.2</v>
+      </c>
+      <c r="T9" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="U9" s="91">
+        <f>1-T10</f>
+        <v>0.5</v>
+      </c>
+      <c r="V9" s="91">
+        <f>1-T11</f>
+        <v>0.8</v>
+      </c>
+      <c r="X9" s="91" t="b">
+        <f>AND(S9&lt;=T9,T9&lt;=U9,U9&lt;=V9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="91">
+        <f>1-G11</f>
+        <v>0.8</v>
+      </c>
+      <c r="J10" s="91" t="b">
+        <f>AND(E10&lt;=F10,F10&lt;=G10,G10&lt;=H10)</f>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>0.2</v>
+      </c>
+      <c r="T10">
+        <v>0.5</v>
+      </c>
+      <c r="U10" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="V10" s="91">
+        <f>1-U11</f>
+        <v>0.8</v>
+      </c>
+      <c r="X10" s="91" t="b">
+        <f>AND(S10&lt;=T10,T10&lt;=U10,U10&lt;=V10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.2</v>
+      </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="91" t="b">
+        <f>AND(E11&lt;=F11,F11&lt;=G11,G11&lt;=H11)</f>
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>0.1</v>
+      </c>
+      <c r="T11">
+        <v>0.2</v>
+      </c>
+      <c r="U11">
+        <v>0.2</v>
+      </c>
+      <c r="V11" s="91">
+        <v>0.5</v>
+      </c>
+      <c r="X11" s="91" t="b">
+        <f>AND(S11&lt;=T11,T11&lt;=U11,U11&lt;=V11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="E13" s="91" t="b">
+        <f>AND(E11&lt;=E10, E10&lt;=E9, E9&lt;=E8)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="91" t="b">
+        <f>AND(F11&lt;=F10, F10&lt;=F9, F9&lt;=F8)</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="91" t="b">
+        <f>AND(G11&lt;=G10, G10&lt;=G9, G9&lt;=G8)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="91" t="b">
+        <f>AND(H11&lt;=H10, H10&lt;=H9, H9&lt;=H8)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <f>AND(E13:H13,J8:J11)</f>
+        <v>1</v>
+      </c>
+      <c r="S13" s="91" t="b">
+        <f>AND(S11&lt;=S10, S10&lt;=S9, S9&lt;=S8)</f>
+        <v>1</v>
+      </c>
+      <c r="T13" s="91" t="b">
+        <f>AND(T11&lt;=T10, T10&lt;=T9, T9&lt;=T8)</f>
+        <v>1</v>
+      </c>
+      <c r="U13" s="91" t="b">
+        <f>AND(U11&lt;=U10, U10&lt;=U9, U9&lt;=U8)</f>
+        <v>1</v>
+      </c>
+      <c r="V13" s="91" t="b">
+        <f>AND(V11&lt;=V10, V10&lt;=V9, V9&lt;=V8)</f>
+        <v>1</v>
+      </c>
+      <c r="X13" t="b">
+        <f>AND(S13:V13,X8:X11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:29" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <v>4</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>2</v>
+      </c>
+      <c r="U16">
+        <v>3</v>
+      </c>
+      <c r="V16">
+        <v>4</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>2</v>
+      </c>
+      <c r="AB16">
+        <v>3</v>
+      </c>
+      <c r="AC16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17">
+        <f>F8</f>
+        <v>0.8</v>
+      </c>
+      <c r="F17">
+        <f>E9</f>
+        <v>0.2</v>
+      </c>
+      <c r="I17">
+        <f>H8*G9</f>
+        <v>0.5</v>
+      </c>
+      <c r="L17">
+        <f>E17*$H17</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17:O20" si="0">F17*$H17</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>133</v>
+      </c>
+      <c r="S17">
+        <f>T8</f>
+        <v>0.8</v>
+      </c>
+      <c r="T17">
+        <f>S9</f>
+        <v>0.2</v>
+      </c>
+      <c r="W17">
+        <f>V8*U9</f>
+        <v>0.45</v>
+      </c>
+      <c r="Z17">
+        <f>S17*$V17</f>
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" ref="AA17:AC20" si="1">T17*$V17</f>
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18">
+        <f>G8</f>
+        <v>0.8</v>
+      </c>
+      <c r="G18">
+        <f>E10</f>
+        <v>0.2</v>
+      </c>
+      <c r="I18">
+        <f>H8*F10</f>
+        <v>0.5</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L20" si="2">E18*$H18</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>134</v>
+      </c>
+      <c r="S18">
+        <f>U8</f>
+        <v>0.8</v>
+      </c>
+      <c r="U18">
+        <f>S10</f>
+        <v>0.2</v>
+      </c>
+      <c r="W18">
+        <f>V8*T10</f>
+        <v>0.45</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" ref="Z18:Z20" si="3">S18*$V18</f>
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19">
+        <f>H9</f>
+        <v>0.8</v>
+      </c>
+      <c r="H19">
+        <f>F11</f>
+        <v>0.2</v>
+      </c>
+      <c r="I19">
+        <f>E11*G9</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="R19" t="s">
+        <v>135</v>
+      </c>
+      <c r="T19">
+        <f>V9</f>
+        <v>0.8</v>
+      </c>
+      <c r="V19">
+        <f>T11</f>
+        <v>0.2</v>
+      </c>
+      <c r="W19">
+        <f>S11*U9</f>
+        <v>0.05</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="1"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20">
+        <f>H10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H20">
+        <f>G11</f>
+        <v>0.2</v>
+      </c>
+      <c r="I20">
+        <f>E11*F10</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="0"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="R20" t="s">
+        <v>136</v>
+      </c>
+      <c r="U20">
+        <f>V10</f>
+        <v>0.8</v>
+      </c>
+      <c r="V20">
+        <f>U11</f>
+        <v>0.2</v>
+      </c>
+      <c r="W20">
+        <f>S11*T10</f>
+        <v>0.05</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="1"/>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <f>SUM(L17:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>SUM(M17:M20)</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="N22">
+        <f>SUM(N17:N20)</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="O22">
+        <f>SUM(O17:O20)</f>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="Z22">
+        <f>SUM(Z17:Z20)</f>
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <f>SUM(AA17:AA20)</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="AB22">
+        <f>SUM(AB17:AB20)</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="AC22">
+        <f>SUM(AC17:AC20)</f>
+        <v>8.0000000000000016E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <f>N22*S10</f>
+        <v>3.2000000000000008E-2</v>
+      </c>
+      <c r="AB24">
+        <f>AB22*E10</f>
+        <v>3.2000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:29" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15037,7 +15689,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="81"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -15045,7 +15697,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="81"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
@@ -15079,7 +15731,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="81"/>
+      <c r="D12" s="82"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -15087,7 +15739,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="81"/>
+      <c r="D13" s="82"/>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
@@ -15121,7 +15773,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="81"/>
+      <c r="D16" s="82"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -15129,7 +15781,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="81"/>
+      <c r="D17" s="82"/>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -15225,7 +15877,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="81"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -15235,7 +15887,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="81"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -15245,32 +15897,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="85" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="87"/>
-      <c r="F10" s="82"/>
+      <c r="F10" s="88"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="83"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="87"/>
-      <c r="F11" s="82"/>
+      <c r="F11" s="88"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="84"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="82"/>
+      <c r="E12" s="88"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -15278,37 +15930,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="85" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="82"/>
+      <c r="E13" s="88"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="83" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="82"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="88"/>
       <c r="E14" s="87"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="85"/>
+      <c r="I14" s="83"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="82"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="88"/>
       <c r="E15" s="87"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="86"/>
+      <c r="I15" s="84"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -15317,7 +15969,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="81"/>
+      <c r="F16" s="82"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -15327,7 +15979,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="81"/>
+      <c r="F17" s="82"/>
       <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
@@ -15365,9 +16017,9 @@
         <v>27</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -15375,9 +16027,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
@@ -15396,17 +16048,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rewrote edwards theorem to use stapling and containment lemmas
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C83B625-F1BE-417E-8334-5C55C9E57AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B54E07-806C-4DEB-9E1E-E50D66834459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="13" activeTab="23" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="16" activeTab="24" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="Sheet21" sheetId="23" r:id="rId22"/>
     <sheet name="Sheet22" sheetId="24" r:id="rId23"/>
     <sheet name="Sheet23" sheetId="25" r:id="rId24"/>
+    <sheet name="Sheet24" sheetId="26" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="144">
   <si>
     <t>Georgia</t>
   </si>
@@ -476,6 +477,21 @@
   </si>
   <si>
     <t>pki*W(x-i)</t>
+  </si>
+  <si>
+    <t>k-1</t>
+  </si>
+  <si>
+    <t>\ell</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>\ell-1</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -948,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1077,8 +1093,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1087,15 +1113,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1104,7 +1121,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7148,16 +7174,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="90"/>
+      <c r="E5" s="91"/>
       <c r="F5" s="67"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="89" t="s">
+      <c r="H5" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="90"/>
+      <c r="I5" s="91"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -9030,7 +9056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DAA05C-8B34-498C-B0AB-56B73244FFB8}">
   <dimension ref="A4:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="C8" workbookViewId="0">
       <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
@@ -11312,8 +11338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887B89AA-C696-4373-8C0A-DD193E62BDA9}">
   <dimension ref="C5:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BM17" sqref="BM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11359,22 +11385,22 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="91">
+      <c r="E8" s="82">
         <v>0.5</v>
       </c>
-      <c r="F8" s="91">
+      <c r="F8" s="82">
         <f>1-E9</f>
         <v>0.8</v>
       </c>
-      <c r="G8" s="91">
+      <c r="G8" s="82">
         <f>1-E10</f>
         <v>0.8</v>
       </c>
-      <c r="H8" s="91">
+      <c r="H8" s="82">
         <f>1-E11</f>
         <v>1</v>
       </c>
-      <c r="J8" s="91" t="b">
+      <c r="J8" s="82" t="b">
         <f>AND(E8&lt;=F8,F8&lt;=G8,G8&lt;=H8)</f>
         <v>1</v>
       </c>
@@ -11384,22 +11410,22 @@
       <c r="R8">
         <v>1</v>
       </c>
-      <c r="S8" s="91">
+      <c r="S8" s="82">
         <v>0.5</v>
       </c>
-      <c r="T8" s="91">
+      <c r="T8" s="82">
         <f>1-S9</f>
         <v>0.8</v>
       </c>
-      <c r="U8" s="91">
+      <c r="U8" s="82">
         <f>1-S10</f>
         <v>0.8</v>
       </c>
-      <c r="V8" s="91">
+      <c r="V8" s="82">
         <f>1-S11</f>
         <v>0.9</v>
       </c>
-      <c r="X8" s="91" t="b">
+      <c r="X8" s="82" t="b">
         <f>AND(S8&lt;=T8,T8&lt;=U8,U8&lt;=V8)</f>
         <v>1</v>
       </c>
@@ -11411,18 +11437,18 @@
       <c r="E9">
         <v>0.2</v>
       </c>
-      <c r="F9" s="91">
+      <c r="F9" s="82">
         <v>0.5</v>
       </c>
-      <c r="G9" s="91">
+      <c r="G9" s="82">
         <f>1-F10</f>
         <v>0.5</v>
       </c>
-      <c r="H9" s="91">
+      <c r="H9" s="82">
         <f>1-F11</f>
         <v>0.8</v>
       </c>
-      <c r="J9" s="91" t="b">
+      <c r="J9" s="82" t="b">
         <f>AND(E9&lt;=F9,F9&lt;=G9,G9&lt;=H9)</f>
         <v>1</v>
       </c>
@@ -11432,18 +11458,18 @@
       <c r="S9">
         <v>0.2</v>
       </c>
-      <c r="T9" s="91">
+      <c r="T9" s="82">
         <v>0.5</v>
       </c>
-      <c r="U9" s="91">
+      <c r="U9" s="82">
         <f>1-T10</f>
         <v>0.5</v>
       </c>
-      <c r="V9" s="91">
+      <c r="V9" s="82">
         <f>1-T11</f>
         <v>0.8</v>
       </c>
-      <c r="X9" s="91" t="b">
+      <c r="X9" s="82" t="b">
         <f>AND(S9&lt;=T9,T9&lt;=U9,U9&lt;=V9)</f>
         <v>1</v>
       </c>
@@ -11458,14 +11484,14 @@
       <c r="F10">
         <v>0.5</v>
       </c>
-      <c r="G10" s="91">
+      <c r="G10" s="82">
         <v>0.5</v>
       </c>
-      <c r="H10" s="91">
+      <c r="H10" s="82">
         <f>1-G11</f>
         <v>0.8</v>
       </c>
-      <c r="J10" s="91" t="b">
+      <c r="J10" s="82" t="b">
         <f>AND(E10&lt;=F10,F10&lt;=G10,G10&lt;=H10)</f>
         <v>1</v>
       </c>
@@ -11478,14 +11504,14 @@
       <c r="T10">
         <v>0.5</v>
       </c>
-      <c r="U10" s="91">
+      <c r="U10" s="82">
         <v>0.5</v>
       </c>
-      <c r="V10" s="91">
+      <c r="V10" s="82">
         <f>1-U11</f>
         <v>0.8</v>
       </c>
-      <c r="X10" s="91" t="b">
+      <c r="X10" s="82" t="b">
         <f>AND(S10&lt;=T10,T10&lt;=U10,U10&lt;=V10)</f>
         <v>1</v>
       </c>
@@ -11503,10 +11529,10 @@
       <c r="G11">
         <v>0.2</v>
       </c>
-      <c r="H11" s="91">
+      <c r="H11" s="82">
         <v>0.5</v>
       </c>
-      <c r="J11" s="91" t="b">
+      <c r="J11" s="82" t="b">
         <f>AND(E11&lt;=F11,F11&lt;=G11,G11&lt;=H11)</f>
         <v>1</v>
       </c>
@@ -11522,28 +11548,28 @@
       <c r="U11">
         <v>0.2</v>
       </c>
-      <c r="V11" s="91">
+      <c r="V11" s="82">
         <v>0.5</v>
       </c>
-      <c r="X11" s="91" t="b">
+      <c r="X11" s="82" t="b">
         <f>AND(S11&lt;=T11,T11&lt;=U11,U11&lt;=V11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:29" x14ac:dyDescent="0.3">
-      <c r="E13" s="91" t="b">
+      <c r="E13" s="82" t="b">
         <f>AND(E11&lt;=E10, E10&lt;=E9, E9&lt;=E8)</f>
         <v>1</v>
       </c>
-      <c r="F13" s="91" t="b">
+      <c r="F13" s="82" t="b">
         <f>AND(F11&lt;=F10, F10&lt;=F9, F9&lt;=F8)</f>
         <v>1</v>
       </c>
-      <c r="G13" s="91" t="b">
+      <c r="G13" s="82" t="b">
         <f>AND(G11&lt;=G10, G10&lt;=G9, G9&lt;=G8)</f>
         <v>1</v>
       </c>
-      <c r="H13" s="91" t="b">
+      <c r="H13" s="82" t="b">
         <f>AND(H11&lt;=H10, H10&lt;=H9, H9&lt;=H8)</f>
         <v>1</v>
       </c>
@@ -11551,19 +11577,19 @@
         <f>AND(E13:H13,J8:J11)</f>
         <v>1</v>
       </c>
-      <c r="S13" s="91" t="b">
+      <c r="S13" s="82" t="b">
         <f>AND(S11&lt;=S10, S10&lt;=S9, S9&lt;=S8)</f>
         <v>1</v>
       </c>
-      <c r="T13" s="91" t="b">
+      <c r="T13" s="82" t="b">
         <f>AND(T11&lt;=T10, T10&lt;=T9, T9&lt;=T8)</f>
         <v>1</v>
       </c>
-      <c r="U13" s="91" t="b">
+      <c r="U13" s="82" t="b">
         <f>AND(U11&lt;=U10, U10&lt;=U9, U9&lt;=U8)</f>
         <v>1</v>
       </c>
-      <c r="V13" s="91" t="b">
+      <c r="V13" s="82" t="b">
         <f>AND(V11&lt;=V10, V10&lt;=V9, V9&lt;=V8)</f>
         <v>1</v>
       </c>
@@ -11929,6 +11955,388 @@
       <c r="AB25" t="s">
         <v>138</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E17185E-9620-4E8C-B11F-4E319B7F5AD2}">
+  <dimension ref="A3:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="11" width="5.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="93">
+        <v>1</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="93" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="93" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="93" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="93">
+        <v>1</v>
+      </c>
+      <c r="C6" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="93" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="95"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="95"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="93" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="95"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="93" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="95"/>
+      <c r="K12" s="95"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="94"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15689,7 +16097,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="82"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -15697,7 +16105,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="82"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
@@ -15731,7 +16139,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="82"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -15739,7 +16147,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="82"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
@@ -15773,7 +16181,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="82"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -15781,7 +16189,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="82"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -15877,7 +16285,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="82"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -15887,7 +16295,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="82"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -15902,8 +16310,8 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="84"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
@@ -15912,8 +16320,8 @@
       <c r="B11" s="85"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="84"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
@@ -15922,7 +16330,7 @@
       <c r="B12" s="86"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="88"/>
+      <c r="E12" s="84"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -15934,33 +16342,33 @@
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="88"/>
+      <c r="E13" s="84"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="83" t="s">
+      <c r="I13" s="87" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="85"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="87"/>
+      <c r="D14" s="84"/>
+      <c r="E14" s="89"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="83"/>
+      <c r="I14" s="87"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
       <c r="C15" s="86"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="87"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="89"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="84"/>
+      <c r="I15" s="88"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -15969,7 +16377,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="82"/>
+      <c r="F16" s="83"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -15979,7 +16387,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="82"/>
+      <c r="F17" s="83"/>
       <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
@@ -16017,9 +16425,9 @@
         <v>27</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -16027,9 +16435,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
@@ -16048,17 +16456,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Moving faithfulness to analytics
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310ABD4-10A1-49B6-9904-CB75273CCA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9083F89-1DC5-4C6C-9A7B-3D9A3B8B1B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="22" activeTab="29" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="16" activeTab="16" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <sheet name="Sheet29" sheetId="31" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="195">
   <si>
     <t>Georgia</t>
   </si>
@@ -609,6 +610,48 @@
   </si>
   <si>
     <t>Emerson</t>
+  </si>
+  <si>
+    <t>1 Collingwood</t>
+  </si>
+  <si>
+    <t>4 Melborne</t>
+  </si>
+  <si>
+    <t>8 Sydney</t>
+  </si>
+  <si>
+    <t>7 GW Sydney</t>
+  </si>
+  <si>
+    <t>2 Brisbaine</t>
+  </si>
+  <si>
+    <t>3 Port Adeliade</t>
+  </si>
+  <si>
+    <t>Collingwood</t>
+  </si>
+  <si>
+    <t>Brisbaine</t>
+  </si>
+  <si>
+    <t>Melborne</t>
+  </si>
+  <si>
+    <t>Port Adeliade</t>
+  </si>
+  <si>
+    <t>5 Carlton</t>
+  </si>
+  <si>
+    <t>Carlton</t>
+  </si>
+  <si>
+    <t>GW Sydney</t>
+  </si>
+  <si>
+    <t>6 St. Kilda</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1498,46 +1541,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1553,21 +1556,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1577,21 +1565,62 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1599,10 +1628,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3809,7 +3837,7 @@
     </row>
     <row r="10" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
-      <c r="D10" s="99" t="s">
+      <c r="D10" s="109" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1"/>
@@ -3818,7 +3846,7 @@
     </row>
     <row r="11" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="64"/>
-      <c r="D11" s="100"/>
+      <c r="D11" s="110"/>
       <c r="E11" s="1"/>
       <c r="F11" s="20"/>
       <c r="G11" s="1"/>
@@ -3864,7 +3892,7 @@
     </row>
     <row r="17" spans="3:7" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
-      <c r="D17" s="99" t="s">
+      <c r="D17" s="109" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="1"/>
@@ -3873,7 +3901,7 @@
     </row>
     <row r="18" spans="3:7" ht="7.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="64"/>
-      <c r="D18" s="100"/>
+      <c r="D18" s="110"/>
       <c r="E18" s="1"/>
       <c r="F18" s="20"/>
       <c r="G18" s="1"/>
@@ -4303,16 +4331,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5E35F-6BAF-409B-A5CF-ACCF63F9A711}">
   <dimension ref="B4:BT40"/>
   <sheetViews>
-    <sheetView topLeftCell="BE4" workbookViewId="0">
-      <selection activeCell="BZ10" sqref="BZ10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="H5:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.77734375" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:72" x14ac:dyDescent="0.3">
@@ -5771,14 +5798,18 @@
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="8" t="s">
         <v>89</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="K19" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="8">
@@ -5871,17 +5902,13 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -5970,17 +5997,17 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="66" t="s">
-        <v>66</v>
+      <c r="E21" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="J21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -6083,17 +6110,17 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="4"/>
+      <c r="E22" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7"/>
+      <c r="K22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K22" s="4"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -6182,13 +6209,17 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="J23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="4"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -10049,16 +10080,16 @@
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="113" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="105"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="67"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="104" t="s">
+      <c r="H5" s="113" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="105"/>
+      <c r="I5" s="114"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -11524,7 +11555,7 @@
   <dimension ref="B2:M35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="B3" sqref="B1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12485,7 +12516,7 @@
         <v>0.5</v>
       </c>
       <c r="L18">
-        <f t="shared" ref="L18:L20" si="2">E18*$H18</f>
+        <f>E18*$H18</f>
         <v>0</v>
       </c>
       <c r="M18">
@@ -12516,7 +12547,7 @@
         <v>0.45</v>
       </c>
       <c r="Z18">
-        <f t="shared" ref="Z18:Z20" si="3">S18*$V18</f>
+        <f>S18*$V18</f>
         <v>0</v>
       </c>
       <c r="AA18">
@@ -12549,7 +12580,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
+        <f>E19*$H19</f>
         <v>0</v>
       </c>
       <c r="M19">
@@ -12580,7 +12611,7 @@
         <v>0.05</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="3"/>
+        <f>S19*$V19</f>
         <v>0</v>
       </c>
       <c r="AA19">
@@ -12613,7 +12644,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <f t="shared" si="2"/>
+        <f>E20*$H20</f>
         <v>0</v>
       </c>
       <c r="M20">
@@ -12644,7 +12675,7 @@
         <v>0.05</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="3"/>
+        <f>S20*$V20</f>
         <v>0</v>
       </c>
       <c r="AA20">
@@ -14715,7 +14746,7 @@
   <dimension ref="C1:T98"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:I8"/>
+      <selection activeCell="F19" sqref="F19:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14751,59 +14782,59 @@
     </row>
     <row r="2" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="121" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="108" t="s">
+      <c r="M2" s="121" t="s">
         <v>95</v>
       </c>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="110"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="123"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="116" t="s">
+      <c r="E3" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="124"/>
+      <c r="F3" s="116"/>
       <c r="G3" s="117"/>
       <c r="H3" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="I3" s="112" t="s">
+      <c r="I3" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="111" t="s">
+      <c r="M3" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="116" t="s">
+      <c r="N3" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="O3" s="124"/>
+      <c r="O3" s="116"/>
       <c r="P3" s="117"/>
       <c r="Q3" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="R3" s="112" t="s">
+      <c r="R3" s="98" t="s">
         <v>148</v>
       </c>
       <c r="S3" s="1"/>
@@ -14811,36 +14842,36 @@
     </row>
     <row r="4" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
-      <c r="D4" s="111">
+      <c r="D4" s="97">
         <v>1</v>
       </c>
-      <c r="E4" s="116" t="s">
+      <c r="E4" s="115" t="s">
         <v>151</v>
       </c>
-      <c r="F4" s="124"/>
+      <c r="F4" s="116"/>
       <c r="G4" s="117"/>
       <c r="H4" s="84">
         <v>2</v>
       </c>
-      <c r="I4" s="112">
+      <c r="I4" s="98">
         <f>4-H4</f>
         <v>2</v>
       </c>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="111">
+      <c r="M4" s="97">
         <v>1</v>
       </c>
-      <c r="N4" s="116" t="s">
+      <c r="N4" s="115" t="s">
         <v>156</v>
       </c>
-      <c r="O4" s="124"/>
+      <c r="O4" s="116"/>
       <c r="P4" s="117"/>
       <c r="Q4" s="84">
         <v>4</v>
       </c>
-      <c r="R4" s="112">
+      <c r="R4" s="98">
         <f>4-Q4</f>
         <v>0</v>
       </c>
@@ -14849,37 +14880,37 @@
     </row>
     <row r="5" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="111">
+      <c r="D5" s="97">
         <v>2</v>
       </c>
-      <c r="E5" s="116" t="s">
+      <c r="E5" s="115" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="124"/>
+      <c r="F5" s="116"/>
       <c r="G5" s="117"/>
       <c r="H5" s="84">
         <v>2</v>
       </c>
-      <c r="I5" s="112">
-        <f t="shared" ref="I5:I7" si="0">4-H5</f>
+      <c r="I5" s="98">
+        <f>4-H5</f>
         <v>2</v>
       </c>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="111">
+      <c r="M5" s="97">
         <v>2</v>
       </c>
-      <c r="N5" s="116" t="s">
+      <c r="N5" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="124"/>
+      <c r="O5" s="116"/>
       <c r="P5" s="117"/>
       <c r="Q5" s="84">
         <v>3</v>
       </c>
-      <c r="R5" s="112">
-        <f t="shared" ref="R5:R7" si="1">4-Q5</f>
+      <c r="R5" s="98">
+        <f>4-Q5</f>
         <v>1</v>
       </c>
       <c r="S5" s="1"/>
@@ -14887,37 +14918,37 @@
     </row>
     <row r="6" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
-      <c r="D6" s="111">
+      <c r="D6" s="97">
         <v>3</v>
       </c>
-      <c r="E6" s="116" t="s">
+      <c r="E6" s="115" t="s">
         <v>153</v>
       </c>
-      <c r="F6" s="124"/>
+      <c r="F6" s="116"/>
       <c r="G6" s="117"/>
       <c r="H6" s="84">
         <v>2</v>
       </c>
-      <c r="I6" s="112">
-        <f t="shared" si="0"/>
+      <c r="I6" s="98">
+        <f>4-H6</f>
         <v>2</v>
       </c>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="111">
+      <c r="M6" s="97">
         <v>3</v>
       </c>
-      <c r="N6" s="116" t="s">
+      <c r="N6" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="124"/>
+      <c r="O6" s="116"/>
       <c r="P6" s="117"/>
       <c r="Q6" s="84">
         <v>2</v>
       </c>
-      <c r="R6" s="112">
-        <f t="shared" si="1"/>
+      <c r="R6" s="98">
+        <f>4-Q6</f>
         <v>2</v>
       </c>
       <c r="S6" s="1"/>
@@ -14925,37 +14956,37 @@
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
-      <c r="D7" s="111">
+      <c r="D7" s="97">
         <v>4</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="115" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="124"/>
+      <c r="F7" s="116"/>
       <c r="G7" s="117"/>
       <c r="H7" s="84">
         <v>2</v>
       </c>
-      <c r="I7" s="112">
-        <f t="shared" si="0"/>
+      <c r="I7" s="98">
+        <f>4-H7</f>
         <v>2</v>
       </c>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="111">
+      <c r="M7" s="97">
         <v>4</v>
       </c>
-      <c r="N7" s="116" t="s">
+      <c r="N7" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="O7" s="124"/>
+      <c r="O7" s="116"/>
       <c r="P7" s="117"/>
       <c r="Q7" s="84">
         <v>1</v>
       </c>
-      <c r="R7" s="112">
-        <f t="shared" si="1"/>
+      <c r="R7" s="98">
+        <f>4-Q7</f>
         <v>3</v>
       </c>
       <c r="S7" s="1"/>
@@ -14963,36 +14994,36 @@
     </row>
     <row r="8" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="1"/>
-      <c r="D8" s="113">
+      <c r="D8" s="99">
         <v>5</v>
       </c>
       <c r="E8" s="118" t="s">
         <v>155</v>
       </c>
-      <c r="F8" s="125"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="114">
+      <c r="F8" s="119"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="100">
         <v>2</v>
       </c>
-      <c r="I8" s="115">
+      <c r="I8" s="101">
         <f>4-H8</f>
         <v>2</v>
       </c>
-      <c r="J8" s="120"/>
-      <c r="K8" s="120"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="113">
+      <c r="M8" s="99">
         <v>5</v>
       </c>
       <c r="N8" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="O8" s="125"/>
-      <c r="P8" s="119"/>
-      <c r="Q8" s="114">
+      <c r="O8" s="119"/>
+      <c r="P8" s="120"/>
+      <c r="Q8" s="100">
         <v>0</v>
       </c>
-      <c r="R8" s="115">
+      <c r="R8" s="101">
         <f>4-Q8</f>
         <v>4</v>
       </c>
@@ -15021,59 +15052,59 @@
     </row>
     <row r="10" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
-      <c r="D10" s="108" t="s">
+      <c r="D10" s="121" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="120"/>
-      <c r="K10" s="120"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="108" t="s">
+      <c r="M10" s="121" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="109"/>
-      <c r="O10" s="109"/>
-      <c r="P10" s="109"/>
-      <c r="Q10" s="109"/>
-      <c r="R10" s="110"/>
+      <c r="N10" s="122"/>
+      <c r="O10" s="122"/>
+      <c r="P10" s="122"/>
+      <c r="Q10" s="122"/>
+      <c r="R10" s="123"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
-      <c r="D11" s="111" t="s">
+      <c r="D11" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="116" t="s">
+      <c r="E11" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="124"/>
+      <c r="F11" s="116"/>
       <c r="G11" s="117"/>
       <c r="H11" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="I11" s="112" t="s">
+      <c r="I11" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="J11" s="120"/>
-      <c r="K11" s="120"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="111" t="s">
+      <c r="M11" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="N11" s="116" t="s">
+      <c r="N11" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="O11" s="124"/>
+      <c r="O11" s="116"/>
       <c r="P11" s="117"/>
       <c r="Q11" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="R11" s="112" t="s">
+      <c r="R11" s="98" t="s">
         <v>148</v>
       </c>
       <c r="S11" s="1"/>
@@ -15081,36 +15112,36 @@
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
-      <c r="D12" s="111">
+      <c r="D12" s="97">
         <v>1</v>
       </c>
-      <c r="E12" s="116" t="s">
+      <c r="E12" s="115" t="s">
         <v>158</v>
       </c>
-      <c r="F12" s="124"/>
+      <c r="F12" s="116"/>
       <c r="G12" s="117"/>
       <c r="H12" s="84">
         <v>3</v>
       </c>
-      <c r="I12" s="112">
+      <c r="I12" s="98">
         <f>4-H12</f>
         <v>1</v>
       </c>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="111">
+      <c r="M12" s="97">
         <v>1</v>
       </c>
-      <c r="N12" s="116" t="s">
+      <c r="N12" s="115" t="s">
         <v>101</v>
       </c>
-      <c r="O12" s="124"/>
+      <c r="O12" s="116"/>
       <c r="P12" s="117"/>
       <c r="Q12" s="84">
         <v>4</v>
       </c>
-      <c r="R12" s="112">
+      <c r="R12" s="98">
         <f>4-Q12</f>
         <v>0</v>
       </c>
@@ -15119,37 +15150,37 @@
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
-      <c r="D13" s="111">
+      <c r="D13" s="97">
         <v>2</v>
       </c>
-      <c r="E13" s="116" t="s">
+      <c r="E13" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="124"/>
+      <c r="F13" s="116"/>
       <c r="G13" s="117"/>
       <c r="H13" s="84">
         <v>3</v>
       </c>
-      <c r="I13" s="112">
-        <f t="shared" ref="I13:I15" si="2">4-H13</f>
+      <c r="I13" s="98">
+        <f>4-H13</f>
         <v>1</v>
       </c>
-      <c r="J13" s="120"/>
-      <c r="K13" s="120"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="111">
+      <c r="M13" s="97">
         <v>2</v>
       </c>
-      <c r="N13" s="116" t="s">
+      <c r="N13" s="115" t="s">
         <v>162</v>
       </c>
-      <c r="O13" s="124"/>
+      <c r="O13" s="116"/>
       <c r="P13" s="117"/>
       <c r="Q13" s="84">
         <v>3</v>
       </c>
-      <c r="R13" s="112">
-        <f t="shared" ref="R13:R15" si="3">4-Q13</f>
+      <c r="R13" s="98">
+        <f>4-Q13</f>
         <v>1</v>
       </c>
       <c r="S13" s="1"/>
@@ -15157,37 +15188,37 @@
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
-      <c r="D14" s="111">
+      <c r="D14" s="97">
         <v>3</v>
       </c>
-      <c r="E14" s="116" t="s">
+      <c r="E14" s="115" t="s">
         <v>159</v>
       </c>
-      <c r="F14" s="124"/>
+      <c r="F14" s="116"/>
       <c r="G14" s="117"/>
       <c r="H14" s="84">
         <v>2</v>
       </c>
-      <c r="I14" s="112">
-        <f t="shared" si="2"/>
+      <c r="I14" s="98">
+        <f>4-H14</f>
         <v>2</v>
       </c>
-      <c r="J14" s="120"/>
-      <c r="K14" s="120"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="111">
+      <c r="M14" s="97">
         <v>3</v>
       </c>
-      <c r="N14" s="116" t="s">
+      <c r="N14" s="115" t="s">
         <v>163</v>
       </c>
-      <c r="O14" s="124"/>
+      <c r="O14" s="116"/>
       <c r="P14" s="117"/>
       <c r="Q14" s="84">
         <v>2</v>
       </c>
-      <c r="R14" s="112">
-        <f t="shared" si="3"/>
+      <c r="R14" s="98">
+        <f>4-Q14</f>
         <v>2</v>
       </c>
       <c r="S14" s="1"/>
@@ -15195,37 +15226,37 @@
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
-      <c r="D15" s="111">
+      <c r="D15" s="97">
         <v>4</v>
       </c>
-      <c r="E15" s="116" t="s">
+      <c r="E15" s="115" t="s">
         <v>160</v>
       </c>
-      <c r="F15" s="124"/>
+      <c r="F15" s="116"/>
       <c r="G15" s="117"/>
       <c r="H15" s="84">
         <v>1</v>
       </c>
-      <c r="I15" s="112">
-        <f t="shared" si="2"/>
+      <c r="I15" s="98">
+        <f>4-H15</f>
         <v>3</v>
       </c>
-      <c r="J15" s="120"/>
-      <c r="K15" s="120"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="111">
+      <c r="M15" s="97">
         <v>4</v>
       </c>
-      <c r="N15" s="116" t="s">
+      <c r="N15" s="115" t="s">
         <v>164</v>
       </c>
-      <c r="O15" s="124"/>
+      <c r="O15" s="116"/>
       <c r="P15" s="117"/>
       <c r="Q15" s="84">
         <v>1</v>
       </c>
-      <c r="R15" s="112">
-        <f t="shared" si="3"/>
+      <c r="R15" s="98">
+        <f>4-Q15</f>
         <v>3</v>
       </c>
       <c r="S15" s="1"/>
@@ -15233,36 +15264,36 @@
     </row>
     <row r="16" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
-      <c r="D16" s="113">
+      <c r="D16" s="99">
         <v>5</v>
       </c>
       <c r="E16" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="F16" s="125"/>
-      <c r="G16" s="119"/>
-      <c r="H16" s="114">
+      <c r="F16" s="119"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="100">
         <v>1</v>
       </c>
-      <c r="I16" s="115">
+      <c r="I16" s="101">
         <f>4-H16</f>
         <v>3</v>
       </c>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="113">
+      <c r="M16" s="99">
         <v>5</v>
       </c>
       <c r="N16" s="118" t="s">
         <v>165</v>
       </c>
-      <c r="O16" s="125"/>
-      <c r="P16" s="119"/>
-      <c r="Q16" s="114">
+      <c r="O16" s="119"/>
+      <c r="P16" s="120"/>
+      <c r="Q16" s="100">
         <v>0</v>
       </c>
-      <c r="R16" s="115">
+      <c r="R16" s="101">
         <f>4-Q16</f>
         <v>4</v>
       </c>
@@ -15313,10 +15344,10 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="126" t="s">
+      <c r="F19" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="127" t="s">
+      <c r="G19" s="1" t="s">
         <v>151</v>
       </c>
       <c r="H19" s="1"/>
@@ -15342,16 +15373,16 @@
       <c r="H20" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="107" t="s">
+      <c r="I20" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J20" s="107"/>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
-      <c r="N20" s="107"/>
-      <c r="O20" s="107"/>
-      <c r="P20" s="107"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -15361,7 +15392,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="105" t="s">
         <v>64</v>
       </c>
       <c r="G21" s="12" t="s">
@@ -15371,11 +15402,11 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -15386,7 +15417,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="106"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="59" t="s">
@@ -15397,9 +15428,9 @@
       </c>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
-      <c r="N22" s="107"/>
-      <c r="O22" s="107"/>
-      <c r="P22" s="107"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -15409,10 +15440,10 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="126" t="s">
+      <c r="F23" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="106" t="s">
+      <c r="G23" s="6" t="s">
         <v>101</v>
       </c>
       <c r="H23" s="6"/>
@@ -15422,8 +15453,8 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="5"/>
-      <c r="O23" s="107"/>
-      <c r="P23" s="107"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -15446,8 +15477,8 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="5"/>
-      <c r="O24" s="107"/>
-      <c r="P24" s="107"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -15457,7 +15488,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="126" t="s">
+      <c r="F25" s="105" t="s">
         <v>130</v>
       </c>
       <c r="G25" s="12" t="s">
@@ -15470,7 +15501,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="5"/>
-      <c r="O25" s="107"/>
+      <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -15482,7 +15513,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="107"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
@@ -15505,10 +15536,10 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="126" t="s">
+      <c r="F27" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="106" t="s">
+      <c r="G27" s="6" t="s">
         <v>156</v>
       </c>
       <c r="H27" s="6"/>
@@ -15519,7 +15550,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="4"/>
       <c r="O27" s="11"/>
-      <c r="P27" s="107"/>
+      <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -15534,16 +15565,16 @@
       <c r="H28" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="I28" s="107" t="s">
+      <c r="I28" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
       <c r="N28" s="5"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -15553,7 +15584,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="126" t="s">
+      <c r="F29" s="105" t="s">
         <v>60</v>
       </c>
       <c r="G29" s="12" t="s">
@@ -15563,11 +15594,11 @@
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
       <c r="N29" s="5"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -15578,7 +15609,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="106"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="59" t="s">
@@ -15590,8 +15621,8 @@
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
       <c r="N30" s="5"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
@@ -15601,10 +15632,10 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="126" t="s">
+      <c r="F31" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="106" t="s">
+      <c r="G31" s="6" t="s">
         <v>158</v>
       </c>
       <c r="H31" s="6"/>
@@ -15613,11 +15644,11 @@
       <c r="K31" s="4"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
@@ -15637,11 +15668,11 @@
       <c r="K32" s="5"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
     </row>
@@ -15649,7 +15680,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="126" t="s">
+      <c r="F33" s="105" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="12" t="s">
@@ -15658,14 +15689,14 @@
       <c r="H33" s="8"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="107"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
-      <c r="P33" s="107"/>
-      <c r="Q33" s="107"/>
-      <c r="R33" s="107"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
@@ -15674,18 +15705,18 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="107"/>
-      <c r="H34" s="106"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="107"/>
-      <c r="O34" s="107"/>
-      <c r="P34" s="107"/>
-      <c r="Q34" s="107"/>
-      <c r="R34" s="107"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
@@ -15694,18 +15725,18 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="107"/>
-      <c r="H35" s="106"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="107"/>
-      <c r="L35" s="107"/>
-      <c r="M35" s="107"/>
-      <c r="N35" s="107"/>
-      <c r="O35" s="107"/>
-      <c r="P35" s="107"/>
-      <c r="Q35" s="107"/>
-      <c r="R35" s="107"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
@@ -15714,18 +15745,18 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="107"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="107"/>
-      <c r="N36" s="107"/>
-      <c r="O36" s="107"/>
-      <c r="P36" s="107"/>
-      <c r="Q36" s="107"/>
-      <c r="R36" s="107"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
@@ -15734,17 +15765,17 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="107"/>
-      <c r="H37" s="107"/>
-      <c r="I37" s="107"/>
-      <c r="J37" s="107"/>
-      <c r="K37" s="107"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="107"/>
-      <c r="N37" s="107"/>
-      <c r="O37" s="107"/>
-      <c r="P37" s="107"/>
-      <c r="Q37" s="107"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
@@ -15754,17 +15785,17 @@
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="107"/>
-      <c r="I38" s="107"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="107"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="107"/>
-      <c r="O38" s="107"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
@@ -15779,12 +15810,12 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="107"/>
-      <c r="M39" s="107"/>
-      <c r="N39" s="107"/>
-      <c r="O39" s="107"/>
-      <c r="P39" s="107"/>
-      <c r="Q39" s="107"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
@@ -16971,26 +17002,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="N13:P13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="N12:P12"/>
     <mergeCell ref="D2:I2"/>
@@ -16999,6 +17010,26 @@
     <mergeCell ref="M10:R10"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="N4:P4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="N13:P13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17174,8 +17205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37BDBFED-732D-45BD-9F43-8A836264F93A}">
   <dimension ref="C1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17214,61 +17245,61 @@
     </row>
     <row r="2" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="121" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="108" t="s">
+      <c r="N2" s="121" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="109"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="110"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="122"/>
+      <c r="Q2" s="122"/>
+      <c r="R2" s="122"/>
+      <c r="S2" s="123"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
     <row r="3" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="116" t="s">
+      <c r="E3" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="124"/>
+      <c r="F3" s="116"/>
       <c r="G3" s="117"/>
       <c r="H3" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="I3" s="116" t="s">
+      <c r="I3" s="115" t="s">
         <v>148</v>
       </c>
-      <c r="J3" s="130"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="111" t="s">
+      <c r="N3" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="116" t="s">
+      <c r="O3" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="P3" s="124"/>
+      <c r="P3" s="116"/>
       <c r="Q3" s="117"/>
       <c r="R3" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="S3" s="112" t="s">
+      <c r="S3" s="98" t="s">
         <v>148</v>
       </c>
       <c r="T3" s="1"/>
@@ -17276,36 +17307,36 @@
     </row>
     <row r="4" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
-      <c r="D4" s="111">
+      <c r="D4" s="97">
         <v>1</v>
       </c>
-      <c r="E4" s="116" t="s">
+      <c r="E4" s="115" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="124"/>
+      <c r="F4" s="116"/>
       <c r="G4" s="117"/>
       <c r="H4" s="84">
         <v>5</v>
       </c>
-      <c r="I4" s="116">
+      <c r="I4" s="115">
         <v>0</v>
       </c>
-      <c r="J4" s="130"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="111">
+      <c r="N4" s="97">
         <v>1</v>
       </c>
-      <c r="O4" s="116" t="s">
+      <c r="O4" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="P4" s="124"/>
+      <c r="P4" s="116"/>
       <c r="Q4" s="117"/>
       <c r="R4" s="84">
         <v>5</v>
       </c>
-      <c r="S4" s="112">
+      <c r="S4" s="98">
         <v>0</v>
       </c>
       <c r="T4" s="1"/>
@@ -17313,36 +17344,36 @@
     </row>
     <row r="5" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="111">
+      <c r="D5" s="97">
         <v>2</v>
       </c>
-      <c r="E5" s="116" t="s">
+      <c r="E5" s="115" t="s">
         <v>170</v>
       </c>
-      <c r="F5" s="124"/>
+      <c r="F5" s="116"/>
       <c r="G5" s="117"/>
       <c r="H5" s="84">
         <v>4</v>
       </c>
-      <c r="I5" s="116">
+      <c r="I5" s="115">
         <v>1</v>
       </c>
-      <c r="J5" s="130"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="111">
+      <c r="N5" s="97">
         <v>2</v>
       </c>
-      <c r="O5" s="116" t="s">
+      <c r="O5" s="115" t="s">
         <v>176</v>
       </c>
-      <c r="P5" s="124"/>
+      <c r="P5" s="116"/>
       <c r="Q5" s="117"/>
       <c r="R5" s="84">
         <v>3</v>
       </c>
-      <c r="S5" s="112">
+      <c r="S5" s="98">
         <v>2</v>
       </c>
       <c r="T5" s="1"/>
@@ -17350,36 +17381,36 @@
     </row>
     <row r="6" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
-      <c r="D6" s="111">
+      <c r="D6" s="97">
         <v>3</v>
       </c>
-      <c r="E6" s="116" t="s">
+      <c r="E6" s="115" t="s">
         <v>171</v>
       </c>
-      <c r="F6" s="124"/>
+      <c r="F6" s="116"/>
       <c r="G6" s="117"/>
       <c r="H6" s="84">
         <v>3</v>
       </c>
-      <c r="I6" s="116">
+      <c r="I6" s="115">
         <v>2</v>
       </c>
-      <c r="J6" s="130"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="111">
+      <c r="N6" s="97">
         <v>3</v>
       </c>
-      <c r="O6" s="116" t="s">
+      <c r="O6" s="115" t="s">
         <v>177</v>
       </c>
-      <c r="P6" s="124"/>
+      <c r="P6" s="116"/>
       <c r="Q6" s="117"/>
       <c r="R6" s="84">
         <v>3</v>
       </c>
-      <c r="S6" s="112">
+      <c r="S6" s="98">
         <v>2</v>
       </c>
       <c r="T6" s="1"/>
@@ -17387,36 +17418,36 @@
     </row>
     <row r="7" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
-      <c r="D7" s="111">
+      <c r="D7" s="97">
         <v>4</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="124"/>
+      <c r="F7" s="116"/>
       <c r="G7" s="117"/>
       <c r="H7" s="84">
         <v>2</v>
       </c>
-      <c r="I7" s="116">
+      <c r="I7" s="115">
         <v>3</v>
       </c>
-      <c r="J7" s="130"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="111">
+      <c r="N7" s="97">
         <v>4</v>
       </c>
-      <c r="O7" s="116" t="s">
+      <c r="O7" s="115" t="s">
         <v>178</v>
       </c>
-      <c r="P7" s="124"/>
+      <c r="P7" s="116"/>
       <c r="Q7" s="117"/>
       <c r="R7" s="84">
         <v>3</v>
       </c>
-      <c r="S7" s="112">
+      <c r="S7" s="98">
         <v>2</v>
       </c>
       <c r="T7" s="1"/>
@@ -17424,36 +17455,36 @@
     </row>
     <row r="8" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
-      <c r="D8" s="123">
+      <c r="D8" s="104">
         <v>5</v>
       </c>
-      <c r="E8" s="116" t="s">
+      <c r="E8" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="124"/>
+      <c r="F8" s="116"/>
       <c r="G8" s="117"/>
-      <c r="H8" s="121">
+      <c r="H8" s="102">
         <v>1</v>
       </c>
-      <c r="I8" s="116">
+      <c r="I8" s="115">
         <v>4</v>
       </c>
-      <c r="J8" s="130"/>
-      <c r="K8" s="120"/>
-      <c r="L8" s="120"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="123">
+      <c r="N8" s="104">
         <v>5</v>
       </c>
-      <c r="O8" s="116" t="s">
+      <c r="O8" s="115" t="s">
         <v>179</v>
       </c>
-      <c r="P8" s="124"/>
+      <c r="P8" s="116"/>
       <c r="Q8" s="117"/>
-      <c r="R8" s="121">
+      <c r="R8" s="102">
         <v>1</v>
       </c>
-      <c r="S8" s="122">
+      <c r="S8" s="103">
         <v>4</v>
       </c>
       <c r="T8" s="1"/>
@@ -17461,36 +17492,36 @@
     </row>
     <row r="9" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="1"/>
-      <c r="D9" s="113">
+      <c r="D9" s="99">
         <v>6</v>
       </c>
       <c r="E9" s="118" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="125"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="114">
+      <c r="F9" s="119"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="100">
         <v>0</v>
       </c>
       <c r="I9" s="118">
         <v>5</v>
       </c>
-      <c r="J9" s="131"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
+      <c r="J9" s="125"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="113">
+      <c r="N9" s="99">
         <v>6</v>
       </c>
       <c r="O9" s="118" t="s">
         <v>180</v>
       </c>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="114">
+      <c r="P9" s="119"/>
+      <c r="Q9" s="120"/>
+      <c r="R9" s="100">
         <v>0</v>
       </c>
-      <c r="S9" s="115">
+      <c r="S9" s="101">
         <v>5</v>
       </c>
       <c r="T9" s="1"/>
@@ -17520,10 +17551,10 @@
     <row r="11" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -17541,10 +17572,10 @@
     <row r="12" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -17562,10 +17593,10 @@
     <row r="13" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="107"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -17583,21 +17614,21 @@
     <row r="14" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
-      <c r="J14" s="107" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K14" s="107"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="107"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107"/>
-      <c r="Q14" s="107"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -17606,19 +17637,19 @@
     <row r="15" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="5"/>
-      <c r="M15" s="107"/>
-      <c r="N15" s="107"/>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -17627,10 +17658,10 @@
     <row r="16" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="106"/>
-      <c r="H16" s="106"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="59" t="s">
@@ -17641,9 +17672,9 @@
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -17653,10 +17684,10 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="126" t="s">
+      <c r="F17" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="6" t="s">
         <v>101</v>
       </c>
       <c r="H17" s="6"/>
@@ -17667,8 +17698,8 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="5"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -17683,7 +17714,7 @@
       <c r="H18" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="129"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="6" t="s">
         <v>97</v>
       </c>
@@ -17692,8 +17723,8 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="107"/>
-      <c r="Q18" s="107"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -17703,7 +17734,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="126" t="s">
+      <c r="F19" s="105" t="s">
         <v>130</v>
       </c>
       <c r="G19" s="12" t="s">
@@ -17717,7 +17748,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="107"/>
+      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -17729,7 +17760,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="107"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="6"/>
@@ -17752,10 +17783,10 @@
     <row r="21" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -17764,7 +17795,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="4"/>
       <c r="P21" s="11"/>
-      <c r="Q21" s="107"/>
+      <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -17773,21 +17804,21 @@
     <row r="22" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="129"/>
-      <c r="I22" s="129"/>
-      <c r="J22" s="107" t="s">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K22" s="107"/>
-      <c r="L22" s="107"/>
-      <c r="M22" s="107"/>
-      <c r="N22" s="107"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
       <c r="O22" s="5"/>
-      <c r="P22" s="107"/>
-      <c r="Q22" s="107"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
@@ -17796,19 +17827,19 @@
     <row r="23" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="106"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="107"/>
-      <c r="N23" s="107"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
       <c r="O23" s="5"/>
-      <c r="P23" s="107"/>
-      <c r="Q23" s="107"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
@@ -17819,7 +17850,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="106"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -17832,8 +17863,8 @@
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
       <c r="O24" s="5"/>
-      <c r="P24" s="107"/>
-      <c r="Q24" s="107"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -17843,10 +17874,10 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="126" t="s">
+      <c r="F25" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="106" t="s">
+      <c r="G25" s="6" t="s">
         <v>158</v>
       </c>
       <c r="H25" s="6"/>
@@ -17856,11 +17887,11 @@
       <c r="L25" s="4"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
     </row>
@@ -17873,7 +17904,7 @@
       <c r="H26" s="66" t="s">
         <v>167</v>
       </c>
-      <c r="I26" s="129"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="6" t="s">
         <v>158</v>
       </c>
@@ -17881,11 +17912,11 @@
       <c r="L26" s="5"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
     </row>
@@ -17893,7 +17924,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="126" t="s">
+      <c r="F27" s="105" t="s">
         <v>92</v>
       </c>
       <c r="G27" s="12" t="s">
@@ -17903,14 +17934,14 @@
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="107"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
     </row>
@@ -17919,19 +17950,19 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
     </row>
@@ -17940,19 +17971,19 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="106"/>
-      <c r="I29" s="106"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
     </row>
@@ -17961,19 +17992,19 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="107"/>
-      <c r="H30" s="107"/>
-      <c r="I30" s="107"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="107"/>
-      <c r="M30" s="107"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
     </row>
@@ -17982,18 +18013,18 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="107"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
@@ -18003,18 +18034,18 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="107"/>
-      <c r="J32" s="107"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -18030,12 +18061,12 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="107"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
-      <c r="P33" s="107"/>
-      <c r="Q33" s="107"/>
-      <c r="R33" s="107"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -19281,12 +19312,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="E6:G6"/>
@@ -19296,14 +19329,12 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="O9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19312,12 +19343,491 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52441B73-D382-4843-A7A3-2711F49B5D63}">
-  <dimension ref="A1"/>
+  <dimension ref="C2:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="6" width="13.44140625" customWidth="1"/>
+    <col min="8" max="10" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+      <c r="D5" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="3:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+      <c r="D9" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="3:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="6">
+        <v>5</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="I14" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="8">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+      <c r="D18" s="6">
+        <v>6</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="D19" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="3:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="1"/>
+      <c r="D20" s="8">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="3:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22983,7 +23493,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="97"/>
+      <c r="D8" s="106"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
@@ -22991,7 +23501,7 @@
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="97"/>
+      <c r="D9" s="106"/>
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
@@ -23025,7 +23535,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="97"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
@@ -23033,7 +23543,7 @@
     <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="97"/>
+      <c r="D13" s="106"/>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
@@ -23067,7 +23577,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="97"/>
+      <c r="D16" s="106"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
@@ -23075,7 +23585,7 @@
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="97"/>
+      <c r="D17" s="106"/>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
@@ -23171,7 +23681,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="97"/>
+      <c r="D8" s="106"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -23181,7 +23691,7 @@
     <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="97"/>
+      <c r="D9" s="106"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
@@ -23191,32 +23701,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="109" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="98"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="112"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="99"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="98"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="112"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="100"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="98"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -23224,37 +23734,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="109" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="98"/>
+      <c r="E13" s="112"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="101" t="s">
+      <c r="I13" s="107" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="103"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="101"/>
+      <c r="I14" s="107"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="103"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="111"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="102"/>
+      <c r="I15" s="108"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -23263,7 +23773,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="97"/>
+      <c r="F16" s="106"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
@@ -23273,7 +23783,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="97"/>
+      <c r="F17" s="106"/>
       <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
@@ -23311,9 +23821,9 @@
         <v>27</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="97"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
@@ -23321,9 +23831,9 @@
     <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="97"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
       <c r="G21" s="1" t="s">
         <v>2</v>
       </c>
@@ -23342,17 +23852,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
WorstCase tiebreaker as a spec
</commit_message>
<xml_diff>
--- a/thesis-tex/images/Brackets.xlsx
+++ b/thesis-tex/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D0994C-C7DA-4D03-802B-D1F5110A4B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B668E333-5608-41EB-8D11-1820E97D8055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="23" activeTab="30" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="23" activeTab="27" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="cfp" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,6 @@
     <definedName name="solver_ver" localSheetId="25" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1597,7 +1596,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1606,13 +1608,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1630,6 +1629,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1639,22 +1647,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -12352,25 +12351,25 @@
     </row>
     <row r="2" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="84"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="87"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="82" t="s">
+      <c r="M2" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="84"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="87"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
@@ -12567,11 +12566,11 @@
       <c r="D8" s="56">
         <v>5</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E8" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="86"/>
-      <c r="G8" s="87"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="84"/>
       <c r="H8" s="57">
         <v>2</v>
       </c>
@@ -12585,11 +12584,11 @@
       <c r="M8" s="56">
         <v>5</v>
       </c>
-      <c r="N8" s="85" t="s">
+      <c r="N8" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="86"/>
-      <c r="P8" s="87"/>
+      <c r="O8" s="83"/>
+      <c r="P8" s="84"/>
       <c r="Q8" s="57">
         <v>0</v>
       </c>
@@ -12622,25 +12621,25 @@
     </row>
     <row r="10" spans="3:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
-      <c r="D10" s="82" t="s">
+      <c r="D10" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="84"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="87"/>
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="82" t="s">
+      <c r="M10" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="N10" s="83"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="83"/>
-      <c r="R10" s="84"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="87"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
@@ -12837,11 +12836,11 @@
       <c r="D16" s="56">
         <v>5</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="86"/>
-      <c r="G16" s="87"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="57">
         <v>1</v>
       </c>
@@ -12855,11 +12854,11 @@
       <c r="M16" s="56">
         <v>5</v>
       </c>
-      <c r="N16" s="85" t="s">
+      <c r="N16" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="O16" s="86"/>
-      <c r="P16" s="87"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="84"/>
       <c r="Q16" s="57">
         <v>0</v>
       </c>
@@ -14572,6 +14571,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="D10:I10"/>
+    <mergeCell ref="M10:R10"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E16:G16"/>
@@ -14586,20 +14599,6 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="N11:P11"/>
     <mergeCell ref="N12:P12"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="M10:R10"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14650,26 +14649,26 @@
     </row>
     <row r="2" spans="3:21" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1"/>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="84"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="82" t="s">
+      <c r="N2" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="84"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="87"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
@@ -14689,7 +14688,7 @@
       <c r="I3" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="89"/>
+      <c r="J3" s="88"/>
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
       <c r="M3" s="1"/>
@@ -14726,7 +14725,7 @@
       <c r="I4" s="79">
         <v>0</v>
       </c>
-      <c r="J4" s="89"/>
+      <c r="J4" s="88"/>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
       <c r="M4" s="1"/>
@@ -14763,7 +14762,7 @@
       <c r="I5" s="79">
         <v>1</v>
       </c>
-      <c r="J5" s="89"/>
+      <c r="J5" s="88"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
       <c r="M5" s="1"/>
@@ -14800,7 +14799,7 @@
       <c r="I6" s="79">
         <v>2</v>
       </c>
-      <c r="J6" s="89"/>
+      <c r="J6" s="88"/>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
       <c r="M6" s="1"/>
@@ -14837,7 +14836,7 @@
       <c r="I7" s="79">
         <v>3</v>
       </c>
-      <c r="J7" s="89"/>
+      <c r="J7" s="88"/>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
       <c r="M7" s="1"/>
@@ -14874,7 +14873,7 @@
       <c r="I8" s="79">
         <v>4</v>
       </c>
-      <c r="J8" s="89"/>
+      <c r="J8" s="88"/>
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
       <c r="M8" s="1"/>
@@ -14900,29 +14899,29 @@
       <c r="D9" s="56">
         <v>6</v>
       </c>
-      <c r="E9" s="85" t="s">
+      <c r="E9" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="86"/>
-      <c r="G9" s="87"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="84"/>
       <c r="H9" s="57">
         <v>0</v>
       </c>
-      <c r="I9" s="85">
+      <c r="I9" s="82">
         <v>5</v>
       </c>
-      <c r="J9" s="90"/>
+      <c r="J9" s="89"/>
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
       <c r="M9" s="1"/>
       <c r="N9" s="56">
         <v>6</v>
       </c>
-      <c r="O9" s="85" t="s">
+      <c r="O9" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="87"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="84"/>
       <c r="R9" s="57">
         <v>0</v>
       </c>
@@ -16717,12 +16716,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="E6:G6"/>
@@ -16732,14 +16733,12 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="O9:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21045,23 +21044,23 @@
     </row>
     <row r="52" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C52">
-        <f t="shared" ref="C52:C83" si="45">IF(AND(D51=D$14,D52=D$13),C$13+C$14-C51,C51)</f>
+        <f t="shared" ref="C52:C78" si="45">IF(AND(D51=D$14,D52=D$13),C$13+C$14-C51,C51)</f>
         <v>2</v>
       </c>
       <c r="D52">
-        <f t="shared" ref="D52:D83" si="46">IF(AND(E51=E$14,E52=E$13),D$13+D$14-D51,D51)</f>
+        <f t="shared" ref="D52:D78" si="46">IF(AND(E51=E$14,E52=E$13),D$13+D$14-D51,D51)</f>
         <v>1</v>
       </c>
       <c r="E52">
-        <f t="shared" ref="E52:E83" si="47">IF(AND(F51=F$14,F52=F$13),E$13+E$14-E51,E51)</f>
+        <f t="shared" ref="E52:E78" si="47">IF(AND(F51=F$14,F52=F$13),E$13+E$14-E51,E51)</f>
         <v>1</v>
       </c>
       <c r="F52">
-        <f t="shared" ref="F52:F83" si="48">IF(AND(G51=G$14,G52=G$13),F$13+F$14-F51,F51)</f>
+        <f t="shared" ref="F52:F78" si="48">IF(AND(G51=G$14,G52=G$13),F$13+F$14-F51,F51)</f>
         <v>3</v>
       </c>
       <c r="G52">
-        <f t="shared" ref="G52:G83" si="49">IF(AND(H51=H$14,H52=H$13),G$13+G$14-G51,G51)</f>
+        <f t="shared" ref="G52:G78" si="49">IF(AND(H51=H$14,H52=H$13),G$13+G$14-G51,G51)</f>
         <v>2</v>
       </c>
       <c r="H52">
@@ -24960,8 +24959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15C56C8-2B90-4EE6-A3F2-D63A46B0A849}">
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25133,7 +25132,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="6" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -25161,7 +25160,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="8" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="1"/>
@@ -29185,7 +29184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602A66C9-975F-464B-97BD-D8A355569D61}">
   <dimension ref="B4:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -34176,32 +34175,32 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="73" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="71"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="76"/>
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="72"/>
+      <c r="B11" s="73"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="71"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="6"/>
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="73"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="71"/>
+      <c r="E12" s="76"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="1"/>
@@ -34209,37 +34208,37 @@
     </row>
     <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="73" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="71"/>
+      <c r="E13" s="76"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="74" t="s">
+      <c r="I13" s="71" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="76"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="75"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="74"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="76"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="75"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="75"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
@@ -34327,17 +34326,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>